<commit_message>
more formatting for supplement tables
</commit_message>
<xml_diff>
--- a/doc/Supplemental_Tables_drafts.xlsx
+++ b/doc/Supplemental_Tables_drafts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="6030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="6030" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="MLH1.M1_models" sheetId="11" r:id="rId1"/>
@@ -40,11 +40,11 @@
     <definedName name="Nrm1CO_Pos_Q1_M3" localSheetId="8">Normalized.Foci.Pos_M2!$A$19:$E$33</definedName>
     <definedName name="PER.IFD_Q1_M2" localSheetId="10">IFD_M2_M3!$M$2:$Q$17</definedName>
     <definedName name="PER.IFD_Q1_M3" localSheetId="10">IFD_M2_M3!$M$21:$Q$36</definedName>
-    <definedName name="ShortSC_Q1_M1" localSheetId="5">Short.bivalent_M1.SC!$A$1:$E$2</definedName>
-    <definedName name="ShortSC_Q1_M1" localSheetId="3">Total.SC.M1!$A$3:$E$4</definedName>
+    <definedName name="ShortSC_Q1_M1" localSheetId="5">Short.bivalent_M1.SC!#REF!</definedName>
+    <definedName name="ShortSC_Q1_M1" localSheetId="3">Total.SC.M1!#REF!</definedName>
     <definedName name="ShortSC_Q1_M2" localSheetId="6">Short.bivalent_M2_M3!$A$2:$E$15</definedName>
-    <definedName name="ShortSC_Q1_M3" localSheetId="6">Short.bivalent_M2_M3!$A$20:$E$33</definedName>
-    <definedName name="ShortSC_Q1_M3" localSheetId="4">Total.SC_M2_M3!$A$22:$E$36</definedName>
+    <definedName name="ShortSC_Q1_M3" localSheetId="6">Short.bivalent_M2_M3!$A$18:$E$31</definedName>
+    <definedName name="ShortSC_Q1_M3" localSheetId="4">Total.SC_M2_M3!$A$20:$E$34</definedName>
     <definedName name="TotalSC_Q1_M2" localSheetId="4">Total.SC_M2_M3!$A$2:$E$17</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -179,29 +179,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="ShortSC_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" tab="0" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="13" name="ShortSC_Q1_M11" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="14" name="ShortSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="12" name="ShortSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -212,7 +190,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="ShortSC_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="13" name="ShortSC_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -223,7 +201,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="ShortSC_Q1_M31" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="14" name="ShortSC_Q1_M31" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -234,7 +212,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="TotalSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="15" name="TotalSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\TotalSC_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -722,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -755,16 +733,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1176,13 +1148,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>195261</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2362200" cy="509820"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="6057900" cy="344453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1190,8 +1162,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="85725" y="376236"/>
-              <a:ext cx="2362200" cy="509820"/>
+              <a:off x="0" y="195261"/>
+              <a:ext cx="6057900" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1242,6 +1214,78 @@
                   </m:oMathParaPr>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                     <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑴</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝟏</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>_</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑨𝑩𝑺</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>_</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑰𝑭𝑫</m:t>
+                    </m:r>
+                    <m:r>
                       <a:rPr lang="en-US" sz="1100" i="1">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
@@ -1464,7 +1508,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1472,8 +1516,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="85725" y="376236"/>
-              <a:ext cx="2362200" cy="509820"/>
+              <a:off x="0" y="195261"/>
+              <a:ext cx="6057900" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1518,12 +1562,24 @@
                 <a:defRPr/>
               </a:pPr>
               <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑴𝟏_𝑨𝑩𝑺_𝑰𝑭𝑫</a:t>
+              </a:r>
+              <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1535,7 +1591,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1547,7 +1603,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1574,14 +1630,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>128586</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>261936</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2790825" cy="509820"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="6029326" cy="344453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1589,8 +1645,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6238874" y="319086"/>
-              <a:ext cx="2790825" cy="509820"/>
+              <a:off x="9515474" y="1214436"/>
+              <a:ext cx="6029326" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1641,6 +1697,78 @@
                   </m:oMathParaPr>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                     <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑴</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝟏</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>_</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑷𝑬𝑹</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>_</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑰𝑭𝑫</m:t>
+                    </m:r>
+                    <m:r>
                       <a:rPr lang="en-US" sz="1100" i="1">
                         <a:solidFill>
                           <a:schemeClr val="tx1"/>
@@ -1887,7 +2015,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1895,8 +2023,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6238874" y="319086"/>
-              <a:ext cx="2790825" cy="509820"/>
+              <a:off x="9515474" y="1214436"/>
+              <a:ext cx="6029326" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1941,7 +2069,7 @@
                 <a:defRPr/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -1950,7 +2078,43 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑚𝑜𝑢𝑠𝑒 𝑎𝑣.</a:t>
+                <a:t>𝑴𝟏_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑷𝑬𝑹</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑰𝑭𝑫</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑚𝑜𝑢𝑠𝑒 𝑎𝑣. </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -1962,7 +2126,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> 𝑁𝑜𝑟𝑚𝑎𝑙𝑖𝑧𝑒𝑑</a:t>
+                <a:t>𝑁𝑜𝑟𝑚𝑎𝑙𝑖𝑧𝑒𝑑</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
@@ -1970,7 +2134,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1982,7 +2146,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1994,7 +2158,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -4586,11 +4750,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
+      <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3133724" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -4598,7 +4762,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="238125"/>
+              <a:off x="0" y="285750"/>
               <a:ext cx="3133724" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4821,7 +4985,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -4829,7 +4993,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="238125"/>
+              <a:off x="0" y="285750"/>
               <a:ext cx="3133724" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4892,11 +5056,11 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> 𝑚𝑜𝑢𝑠𝑒 𝑎𝑣.</a:t>
+                <a:t> 𝑚𝑜𝑢𝑠𝑒 𝑎𝑣.  </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -4908,7 +5072,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>  𝑀𝐿𝐻1</a:t>
+                <a:t>𝑀𝐿𝐻1  = </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
@@ -4916,11 +5080,11 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>  = 𝑠𝑢𝑏𝑠𝑝∗𝑠𝑡𝑟𝑎𝑖𝑛+𝜀</a:t>
+                <a:t>𝑠𝑢𝑏𝑠𝑝∗𝑠𝑡𝑟𝑎𝑖𝑛+𝜀</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100">
                 <a:solidFill>
@@ -5636,13 +5800,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>261936</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1590675" cy="675185"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="6657975" cy="344453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -5650,8 +5814,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="171450" y="1328736"/>
-              <a:ext cx="1590675" cy="675185"/>
+              <a:off x="152400" y="1214436"/>
+              <a:ext cx="6657975" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5948,7 +6112,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -5956,8 +6120,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="171450" y="1328736"/>
-              <a:ext cx="1590675" cy="675185"/>
+              <a:off x="152400" y="1214436"/>
+              <a:ext cx="6657975" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6007,7 +6171,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -6031,7 +6195,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -6066,11 +6230,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>244608</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3381374" cy="509820"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4876800" cy="344453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -6078,8 +6242,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="161925"/>
-              <a:ext cx="3381374" cy="509820"/>
+              <a:off x="0" y="244608"/>
+              <a:ext cx="4876800" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6353,7 +6517,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -6361,8 +6525,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="161925"/>
-              <a:ext cx="3381374" cy="509820"/>
+              <a:off x="0" y="244608"/>
+              <a:ext cx="4876800" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6412,7 +6576,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -6436,7 +6600,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -6465,11 +6629,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2514600" cy="337593"/>
+    <xdr:ext cx="4524375" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -6479,8 +6643,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="28575" y="104775"/>
-              <a:ext cx="2514600" cy="337593"/>
+              <a:off x="9524" y="4210050"/>
+              <a:ext cx="4524375" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6734,8 +6898,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="28575" y="104775"/>
-              <a:ext cx="2514600" cy="337593"/>
+              <a:off x="9524" y="4210050"/>
+              <a:ext cx="4524375" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6839,13 +7003,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1590675" cy="675185"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4838700" cy="344453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -6853,8 +7017,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="171450" y="500061"/>
-              <a:ext cx="1590675" cy="675185"/>
+              <a:off x="1" y="185736"/>
+              <a:ext cx="4838700" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7175,7 +7339,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -7183,8 +7347,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="171450" y="500061"/>
-              <a:ext cx="1590675" cy="675185"/>
+              <a:off x="1" y="185736"/>
+              <a:ext cx="4838700" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7234,7 +7398,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -7258,7 +7422,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -7293,9 +7457,9 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4562474" cy="344453"/>
+    <xdr:ext cx="4514850" cy="344453"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -7305,8 +7469,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="85725"/>
-              <a:ext cx="4562474" cy="344453"/>
+              <a:off x="0" y="152400"/>
+              <a:ext cx="4514850" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7612,8 +7776,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="85725"/>
-              <a:ext cx="4562474" cy="344453"/>
+              <a:off x="0" y="152400"/>
+              <a:ext cx="4514850" cy="344453"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7716,11 +7880,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4429124" cy="172227"/>
+    <xdr:ext cx="3581400" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -7730,8 +7894,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4057650"/>
-              <a:ext cx="4429124" cy="172227"/>
+              <a:off x="200025" y="3562350"/>
+              <a:ext cx="3581400" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8009,8 +8173,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4057650"/>
-              <a:ext cx="4429124" cy="172227"/>
+              <a:off x="200025" y="3562350"/>
+              <a:ext cx="3581400" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9328,34 +9492,26 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M2" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M2" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M2" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M3" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M3" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -9376,19 +9532,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TotalSC_Q1_M2" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TotalSC_Q1_M2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9676,12 +9832,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -9695,7 +9851,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B4">
@@ -9707,10 +9863,10 @@
       <c r="E4" s="7">
         <v>26.356000000000002</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B5">
@@ -9722,10 +9878,10 @@
       <c r="E5" s="7">
         <v>-0.755</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B6">
@@ -9737,10 +9893,10 @@
       <c r="E6" s="7">
         <v>-0.48199999999999998</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B7">
@@ -9753,34 +9909,34 @@
       <c r="E7" s="7">
         <v>-2.649</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="22"/>
       <c r="D8" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="7">
         <v>2.9529999999999998</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="22"/>
       <c r="D9" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="7">
         <v>3.2010000000000001</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <v>1.69</v>
       </c>
     </row>
@@ -9789,13 +9945,13 @@
         <v>33</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <v>1.89</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -9887,408 +10043,405 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="42" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="E2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="7" t="s">
+      <c r="M2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="B3">
         <v>0.12844287037835708</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="7" t="s">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>57.460999999999999</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I2">
+      <c r="J3">
         <v>3.0744844347133315E-2</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>0.47497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>2.6016154168898166E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>-0.71299999999999997</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4">
+        <v>9.0757073711334884E-12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4">
+        <v>6.0099999999999997E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>8.3628920849619676E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>2.9319999999999999</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5">
+        <v>4.6655254665265135E-2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5">
+        <v>-2.8400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>0.40939999999999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>-6.68</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6">
+        <v>0.24440000000000001</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <v>6.9409999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>7.3639999999999999</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7">
+        <v>5.2240000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>-4.5359999999999996</v>
+      </c>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8">
+        <v>-8.1399999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9">
+        <v>8.8800000000000007E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10">
+        <v>7.78</v>
+      </c>
+      <c r="L10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10">
+        <v>4.7989999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="4"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>-4.5359999999999996</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I22" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I23" s="5">
+        <v>-8.1399999999999997E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>83</v>
       </c>
-      <c r="L2" t="s">
+      <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="M2" t="s">
+      <c r="C24" t="s">
         <v>85</v>
       </c>
-      <c r="N2" t="s">
+      <c r="D24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.12844287037835708</v>
+      </c>
+      <c r="B25">
         <v>2.6016154168898166E-2</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3">
+      <c r="C25">
+        <v>8.3628920849619676E-2</v>
+      </c>
+      <c r="D25">
+        <v>0.40939999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" t="s">
+        <v>85</v>
+      </c>
+      <c r="L29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>3.0744844347133315E-2</v>
+      </c>
+      <c r="J30">
         <v>9.0757073711334884E-12</v>
       </c>
-      <c r="K3">
+      <c r="K30">
+        <v>4.6655254665265135E-2</v>
+      </c>
+      <c r="L30">
+        <v>0.24440000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" t="s">
+        <v>84</v>
+      </c>
+      <c r="K32" t="s">
+        <v>85</v>
+      </c>
+      <c r="L32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I33">
         <v>3.0744844347133315E-2</v>
       </c>
-      <c r="L3">
+      <c r="J33">
         <v>9.0757073711334884E-12</v>
       </c>
-      <c r="M3">
+      <c r="K33">
         <v>4.6655254665265135E-2</v>
       </c>
-      <c r="N3">
+      <c r="L33">
         <v>0.24440000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>8.3628920849619676E-2</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4">
-        <v>4.6655254665265135E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5">
-        <v>0.40939999999999999</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5">
-        <v>0.24440000000000001</v>
-      </c>
-      <c r="K5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="K6">
-        <v>3.0744844347133315E-2</v>
-      </c>
-      <c r="L6">
-        <v>9.0757073711334884E-12</v>
-      </c>
-      <c r="M6">
-        <v>4.6655254665265135E-2</v>
-      </c>
-      <c r="N6">
-        <v>0.24440000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8">
-        <v>57.460999999999999</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8">
-        <v>0.47497</v>
-      </c>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>-0.71299999999999997</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9">
-        <v>6.0099999999999997E-3</v>
-      </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>2.9319999999999999</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10">
-        <v>-2.8400000000000001E-3</v>
-      </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11">
-        <v>-6.68</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11">
-        <v>6.9409999999999999E-2</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12">
-        <v>7.3639999999999999</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12">
-        <v>5.2240000000000002E-2</v>
-      </c>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13">
-        <v>-4.5359999999999996</v>
-      </c>
-      <c r="G13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13">
-        <v>-8.1399999999999997E-3</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14">
-        <v>8.8800000000000007E-3</v>
-      </c>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15">
-        <v>7.78</v>
-      </c>
-      <c r="G15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15">
-        <v>4.7989999999999998E-2</v>
-      </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>-4.5359999999999996</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="5">
-        <v>-8.1399999999999997E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>0.12844287037835708</v>
-      </c>
-      <c r="B30">
-        <v>2.6016154168898166E-2</v>
-      </c>
-      <c r="C30">
-        <v>8.3628920849619676E-2</v>
-      </c>
-      <c r="D30">
-        <v>0.40939999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10323,16 +10476,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -11307,16 +11460,16 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -12321,11 +12474,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -12869,11 +13022,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -13430,8 +13583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13442,9 +13595,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -13608,11 +13763,11 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -13772,9 +13927,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -14004,11 +14161,11 @@
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -14233,10 +14390,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A39:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14248,248 +14405,245 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:14" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="B3">
         <v>8.4827723785348087E-4</v>
       </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="7" t="s">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>1960.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3">
+      <c r="B4">
         <v>2.5573249466384537E-31</v>
       </c>
-      <c r="E3">
-        <v>8.4827723785348087E-4</v>
-      </c>
-      <c r="F3">
-        <v>2.5573249466384537E-31</v>
-      </c>
-      <c r="G3">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>-44.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
         <v>9.9096899770360542E-5</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>9.9096899770360542E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="7" t="s">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>-119.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>52</v>
+      <c r="B6">
+        <f>1/10000</f>
+        <v>1E-4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>-558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>167.1</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>396.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="C8">
-        <v>1960.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>-44.1</v>
+      <c r="F9" s="7">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>-119.1</v>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="7">
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11">
-        <v>-558</v>
-      </c>
+      <c r="D11" s="7"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12">
-        <v>167.1</v>
-      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13">
-        <v>396.9</v>
-      </c>
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="7">
-        <v>119</v>
-      </c>
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="7">
-        <v>263</v>
-      </c>
+      <c r="A15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
+      <c r="A16" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="K17" s="11"/>
-      <c r="L17" s="13"/>
+      <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>90</v>
+      <c r="A22" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>70</v>
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>91</v>
+      <c r="A27">
+        <v>8.4827723785348087E-4</v>
+      </c>
+      <c r="B27">
+        <v>2.5573249466384537E-31</v>
+      </c>
+      <c r="C27">
+        <v>9.9096899770360542E-5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14499,10 +14653,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14516,9 +14670,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -14536,7 +14692,7 @@
       <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="15"/>
       <c r="I2" t="s">
         <v>0</v>
       </c>
@@ -14566,7 +14722,7 @@
       <c r="E3" s="6">
         <v>6.8476448906856882E-83</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
         <v>4</v>
@@ -14600,7 +14756,7 @@
       <c r="E4" s="6">
         <v>3.1331650862026381E-4</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="19"/>
       <c r="H4" t="s">
         <v>105</v>
       </c>
@@ -14633,7 +14789,7 @@
       <c r="E5" s="6">
         <v>2.9994818416794007E-3</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="20"/>
       <c r="H5" t="s">
         <v>106</v>
       </c>
@@ -14666,7 +14822,7 @@
       <c r="E6" s="6">
         <v>7.8263498735992003E-13</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
         <v>92</v>
@@ -14700,7 +14856,7 @@
       <c r="E7" s="6">
         <v>5.9726584202964396E-5</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="H7" t="s">
         <v>93</v>
       </c>
@@ -14733,7 +14889,7 @@
       <c r="E8" s="6">
         <v>0.66364908711553217</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="20"/>
       <c r="H8" t="s">
         <v>94</v>
       </c>
@@ -14766,7 +14922,7 @@
       <c r="E9" s="6">
         <v>0.58049315316905858</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="20"/>
       <c r="H9" t="s">
         <v>96</v>
       </c>
@@ -14799,7 +14955,7 @@
       <c r="E10" s="6">
         <v>2.5617511159882357E-8</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="20"/>
       <c r="H10" t="s">
         <v>98</v>
       </c>
@@ -14832,7 +14988,7 @@
       <c r="E11" s="6">
         <v>0.34616907888281573</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="21"/>
       <c r="H11" t="s">
         <v>107</v>
       </c>
@@ -14865,7 +15021,7 @@
       <c r="E12" s="6">
         <v>1.3470832207404887E-2</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="20"/>
       <c r="H12" t="s">
         <v>108</v>
       </c>
@@ -14898,7 +15054,7 @@
       <c r="E13" s="6">
         <v>4.3552294070361525E-4</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="20"/>
       <c r="H13" t="s">
         <v>99</v>
       </c>
@@ -14931,7 +15087,7 @@
       <c r="E14" s="6">
         <v>7.3796863466524351E-2</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="21"/>
       <c r="H14" t="s">
         <v>100</v>
       </c>
@@ -14964,7 +15120,7 @@
       <c r="E15" s="6">
         <v>0.19381122451147587</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="20"/>
       <c r="H15" t="s">
         <v>101</v>
       </c>
@@ -14997,7 +15153,7 @@
       <c r="E16" s="6">
         <v>0.32588118321571224</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="20"/>
       <c r="H16" t="s">
         <v>103</v>
       </c>
@@ -15019,510 +15175,512 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="22"/>
+      <c r="F17" s="20"/>
+    </row>
+    <row r="19" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="I20" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-    </row>
-    <row r="22" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="17"/>
-      <c r="I22" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>1</v>
-      </c>
-      <c r="K22" t="s">
-        <v>2</v>
-      </c>
-      <c r="L22" t="s">
-        <v>3</v>
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1683.3833132361683</v>
+      </c>
+      <c r="C21" s="6">
+        <v>36.478717942393459</v>
+      </c>
+      <c r="D21" s="6">
+        <v>46.146997706842036</v>
+      </c>
+      <c r="E21" s="6">
+        <v>6.8476448906858828E-83</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="H21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>1683.3833132361683</v>
+      </c>
+      <c r="J21">
+        <v>36.478717942393459</v>
+      </c>
+      <c r="K21">
+        <v>46.146997706842036</v>
+      </c>
+      <c r="L21">
+        <v>6.8476448906858828E-83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6">
+        <v>431.23773156183876</v>
+      </c>
+      <c r="C22" s="6">
+        <v>54.282069352294059</v>
+      </c>
+      <c r="D22" s="6">
+        <v>7.9443863638115682</v>
+      </c>
+      <c r="E22" s="6">
+        <v>7.8263498735992003E-13</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="H22" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22">
+        <v>431.23773156183876</v>
+      </c>
+      <c r="J22">
+        <v>54.282069352294059</v>
+      </c>
+      <c r="K22">
+        <v>7.9443863638115682</v>
+      </c>
+      <c r="L22">
+        <v>7.8263498735992003E-13</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B23" s="6">
-        <v>1683.3833132361683</v>
+        <v>248.68440089332017</v>
       </c>
       <c r="C23" s="6">
-        <v>36.478717942393459</v>
+        <v>59.940650057752009</v>
       </c>
       <c r="D23" s="6">
-        <v>46.146997706842036</v>
+        <v>4.1488439089952491</v>
       </c>
       <c r="E23" s="6">
-        <v>6.8476448906858828E-83</v>
-      </c>
-      <c r="F23" s="9"/>
+        <v>5.9726584202965006E-5</v>
+      </c>
+      <c r="F23" s="6"/>
       <c r="H23" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="I23">
-        <v>1683.3833132361683</v>
+        <v>248.68440089332017</v>
       </c>
       <c r="J23">
-        <v>36.478717942393459</v>
+        <v>59.940650057752009</v>
       </c>
       <c r="K23">
-        <v>46.146997706842036</v>
+        <v>4.1488439089952491</v>
       </c>
       <c r="L23">
-        <v>6.8476448906858828E-83</v>
+        <v>5.9726584202965006E-5</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B24" s="6">
-        <v>431.23773156183876</v>
+        <v>202.80451985914706</v>
       </c>
       <c r="C24" s="6">
-        <v>54.282069352294059</v>
+        <v>50.867141869353283</v>
       </c>
       <c r="D24" s="6">
-        <v>7.9443863638115682</v>
+        <v>3.9869454505627306</v>
       </c>
       <c r="E24" s="6">
-        <v>7.8263498735992003E-13</v>
+        <v>1.1061696628946535E-4</v>
       </c>
       <c r="F24" s="6"/>
       <c r="H24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I24">
-        <v>431.23773156183876</v>
+        <v>202.80451985914706</v>
       </c>
       <c r="J24">
-        <v>54.282069352294059</v>
+        <v>50.867141869353283</v>
       </c>
       <c r="K24">
-        <v>7.9443863638115682</v>
+        <v>3.9869454505627306</v>
       </c>
       <c r="L24">
-        <v>7.8263498735992003E-13</v>
+        <v>1.1061696628946535E-4</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B25" s="6">
-        <v>248.68440089332017</v>
+        <v>161.13700122803425</v>
       </c>
       <c r="C25" s="6">
-        <v>59.940650057752009</v>
+        <v>53.280577829112907</v>
       </c>
       <c r="D25" s="6">
-        <v>4.1488439089952491</v>
+        <v>3.0243103170699435</v>
       </c>
       <c r="E25" s="6">
-        <v>5.9726584202965006E-5</v>
+        <v>2.9994818416794332E-3</v>
       </c>
       <c r="F25" s="6"/>
       <c r="H25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I25">
-        <v>248.68440089332017</v>
+        <v>161.13700122803425</v>
       </c>
       <c r="J25">
-        <v>59.940650057752009</v>
+        <v>53.280577829112907</v>
       </c>
       <c r="K25">
-        <v>4.1488439089952491</v>
+        <v>3.0243103170699435</v>
       </c>
       <c r="L25">
-        <v>5.9726584202965006E-5</v>
+        <v>2.9994818416794332E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B26" s="6">
-        <v>202.80451985914706</v>
+        <v>279.64402738196219</v>
       </c>
       <c r="C26" s="6">
-        <v>50.867141869353283</v>
+        <v>83.583243112980881</v>
       </c>
       <c r="D26" s="6">
-        <v>3.9869454505627306</v>
+        <v>3.3456948661822397</v>
       </c>
       <c r="E26" s="6">
-        <v>1.1061696628946535E-4</v>
+        <v>1.0711197146456059E-3</v>
       </c>
       <c r="F26" s="6"/>
       <c r="H26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I26">
-        <v>202.80451985914706</v>
+        <v>279.64402738196219</v>
       </c>
       <c r="J26">
-        <v>50.867141869353283</v>
+        <v>83.583243112980881</v>
       </c>
       <c r="K26">
-        <v>3.9869454505627306</v>
+        <v>3.3456948661822397</v>
       </c>
       <c r="L26">
-        <v>1.1061696628946535E-4</v>
+        <v>1.0711197146456059E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B27" s="6">
-        <v>161.13700122803425</v>
+        <v>229.56811863214378</v>
       </c>
       <c r="C27" s="6">
-        <v>53.280577829112907</v>
+        <v>62.001898206370498</v>
       </c>
       <c r="D27" s="6">
-        <v>3.0243103170699435</v>
+        <v>3.7025982312353847</v>
       </c>
       <c r="E27" s="6">
-        <v>2.9994818416794332E-3</v>
+        <v>3.1331650862026522E-4</v>
       </c>
       <c r="F27" s="6"/>
       <c r="H27" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I27">
-        <v>161.13700122803425</v>
+        <v>229.56811863214378</v>
       </c>
       <c r="J27">
-        <v>53.280577829112907</v>
+        <v>62.001898206370498</v>
       </c>
       <c r="K27">
-        <v>3.0243103170699435</v>
+        <v>3.7025982312353847</v>
       </c>
       <c r="L27">
-        <v>2.9994818416794332E-3</v>
+        <v>3.1331650862026522E-4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6">
-        <v>279.64402738196219</v>
+        <v>-345.00471099408156</v>
       </c>
       <c r="C28" s="6">
-        <v>83.583243112980881</v>
+        <v>58.199900153131772</v>
       </c>
       <c r="D28" s="6">
-        <v>3.3456948661822397</v>
+        <v>-5.9279261663048857</v>
       </c>
       <c r="E28" s="6">
-        <v>1.0711197146456059E-3</v>
-      </c>
-      <c r="F28" s="6"/>
+        <v>2.5617511159882205E-8</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="2"/>
       <c r="H28" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I28">
-        <v>279.64402738196219</v>
+        <v>-345.00471099408156</v>
       </c>
       <c r="J28">
-        <v>83.583243112980881</v>
+        <v>58.199900153131772</v>
       </c>
       <c r="K28">
-        <v>3.3456948661822397</v>
+        <v>-5.9279261663048857</v>
       </c>
       <c r="L28">
-        <v>1.0711197146456059E-3</v>
+        <v>2.5617511159882205E-8</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B29" s="6">
-        <v>229.56811863214378</v>
+        <v>-303.27043531113674</v>
       </c>
       <c r="C29" s="6">
-        <v>62.001898206370498</v>
+        <v>84.021462040331556</v>
       </c>
       <c r="D29" s="6">
-        <v>3.7025982312353847</v>
+        <v>-3.6094401114510766</v>
       </c>
       <c r="E29" s="6">
-        <v>3.1331650862026522E-4</v>
+        <v>4.3552294070361888E-4</v>
       </c>
       <c r="F29" s="6"/>
       <c r="H29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I29">
-        <v>229.56811863214378</v>
+        <v>-303.27043531113674</v>
       </c>
       <c r="J29">
-        <v>62.001898206370498</v>
+        <v>84.021462040331556</v>
       </c>
       <c r="K29">
-        <v>3.7025982312353847</v>
+        <v>-3.6094401114510766</v>
       </c>
       <c r="L29">
-        <v>3.1331650862026522E-4</v>
+        <v>4.3552294070361888E-4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B30" s="6">
-        <v>-345.00471099408156</v>
+        <v>-169.84842882083234</v>
       </c>
       <c r="C30" s="6">
-        <v>58.199900153131772</v>
+        <v>94.239617069217857</v>
       </c>
       <c r="D30" s="6">
-        <v>-5.9279261663048857</v>
+        <v>-1.8023038940839575</v>
       </c>
       <c r="E30" s="6">
-        <v>2.5617511159882205E-8</v>
-      </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="2"/>
+        <v>7.3796863466524643E-2</v>
+      </c>
+      <c r="F30" s="6"/>
       <c r="H30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I30">
-        <v>-345.00471099408156</v>
+        <v>-169.84842882083234</v>
       </c>
       <c r="J30">
-        <v>58.199900153131772</v>
+        <v>94.239617069217857</v>
       </c>
       <c r="K30">
-        <v>-5.9279261663048857</v>
+        <v>-1.8023038940839575</v>
       </c>
       <c r="L30">
-        <v>2.5617511159882205E-8</v>
+        <v>7.3796863466524643E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B31" s="6">
-        <v>-303.27043531113674</v>
+        <v>37.167574701963318</v>
       </c>
       <c r="C31" s="6">
-        <v>84.021462040331556</v>
+        <v>86.439160513925671</v>
       </c>
       <c r="D31" s="6">
-        <v>-3.6094401114510766</v>
+        <v>0.42998537330745457</v>
       </c>
       <c r="E31" s="6">
-        <v>4.3552294070361888E-4</v>
+        <v>0.66791276924653886</v>
       </c>
       <c r="F31" s="6"/>
       <c r="H31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I31">
-        <v>-303.27043531113674</v>
+        <v>37.167574701963318</v>
       </c>
       <c r="J31">
-        <v>84.021462040331556</v>
+        <v>86.439160513925671</v>
       </c>
       <c r="K31">
-        <v>-3.6094401114510766</v>
+        <v>0.42998537330745457</v>
       </c>
       <c r="L31">
-        <v>4.3552294070361888E-4</v>
+        <v>0.66791276924653886</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B32" s="6">
-        <v>-169.84842882083234</v>
+        <v>243.12526191449476</v>
       </c>
       <c r="C32" s="6">
-        <v>94.239617069217857</v>
+        <v>97.055246237224836</v>
       </c>
       <c r="D32" s="6">
-        <v>-1.8023038940839575</v>
+        <v>2.5050192683066506</v>
       </c>
       <c r="E32" s="6">
-        <v>7.3796863466524643E-2</v>
+        <v>1.347083220740479E-2</v>
       </c>
       <c r="F32" s="6"/>
       <c r="H32" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I32">
-        <v>-169.84842882083234</v>
+        <v>243.12526191449476</v>
       </c>
       <c r="J32">
-        <v>94.239617069217857</v>
+        <v>97.055246237224836</v>
       </c>
       <c r="K32">
-        <v>-1.8023038940839575</v>
+        <v>2.5050192683066506</v>
       </c>
       <c r="L32">
-        <v>7.3796863466524643E-2</v>
+        <v>1.347083220740479E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B33" s="6">
-        <v>37.167574701963318</v>
+        <v>-204.10391480119597</v>
       </c>
       <c r="C33" s="6">
-        <v>86.439160513925671</v>
+        <v>116.47772052048346</v>
       </c>
       <c r="D33" s="6">
-        <v>0.42998537330745457</v>
+        <v>-1.7523000440698253</v>
       </c>
       <c r="E33" s="6">
-        <v>0.66791276924653886</v>
+        <v>8.2062013862105154E-2</v>
       </c>
       <c r="F33" s="6"/>
       <c r="H33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I33">
-        <v>37.167574701963318</v>
+        <v>-204.10391480119597</v>
       </c>
       <c r="J33">
-        <v>86.439160513925671</v>
+        <v>116.47772052048346</v>
       </c>
       <c r="K33">
-        <v>0.42998537330745457</v>
+        <v>-1.7523000440698253</v>
       </c>
       <c r="L33">
-        <v>0.66791276924653886</v>
+        <v>8.2062013862105154E-2</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B34" s="6">
-        <v>243.12526191449476</v>
+        <v>-84.337752392824129</v>
       </c>
       <c r="C34" s="6">
-        <v>97.055246237224836</v>
+        <v>89.203690570630229</v>
       </c>
       <c r="D34" s="6">
-        <v>2.5050192683066506</v>
+        <v>-0.9454513804677922</v>
       </c>
       <c r="E34" s="6">
-        <v>1.347083220740479E-2</v>
+        <v>0.34616907888281784</v>
       </c>
       <c r="F34" s="6"/>
       <c r="H34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I34">
-        <v>243.12526191449476</v>
+        <v>-84.337752392824129</v>
       </c>
       <c r="J34">
-        <v>97.055246237224836</v>
+        <v>89.203690570630229</v>
       </c>
       <c r="K34">
-        <v>2.5050192683066506</v>
+        <v>-0.9454513804677922</v>
       </c>
       <c r="L34">
-        <v>1.347083220740479E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="6">
-        <v>-204.10391480119597</v>
-      </c>
-      <c r="C35" s="6">
-        <v>116.47772052048346</v>
-      </c>
-      <c r="D35" s="6">
-        <v>-1.7523000440698253</v>
-      </c>
-      <c r="E35" s="6">
-        <v>8.2062013862105154E-2</v>
-      </c>
-      <c r="F35" s="6"/>
-      <c r="H35" t="s">
-        <v>103</v>
-      </c>
-      <c r="I35">
-        <v>-204.10391480119597</v>
-      </c>
-      <c r="J35">
-        <v>116.47772052048346</v>
-      </c>
-      <c r="K35">
-        <v>-1.7523000440698253</v>
-      </c>
-      <c r="L35">
-        <v>8.2062013862105154E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="6">
-        <v>-84.337752392824129</v>
-      </c>
-      <c r="C36" s="6">
-        <v>89.203690570630229</v>
-      </c>
-      <c r="D36" s="6">
-        <v>-0.9454513804677922</v>
-      </c>
-      <c r="E36" s="6">
-        <v>0.34616907888281784</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="H36" t="s">
-        <v>104</v>
-      </c>
-      <c r="I36">
-        <v>-84.337752392824129</v>
-      </c>
-      <c r="J36">
-        <v>89.203690570630229</v>
-      </c>
-      <c r="K36">
-        <v>-0.9454513804677922</v>
-      </c>
-      <c r="L36">
         <v>0.34616907888281784</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15531,201 +15689,226 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
         <v>0.12683705033364417</v>
       </c>
-      <c r="F2">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="15">
+        <v>80.34</v>
+      </c>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
         <v>1.1225128823082477E-11</v>
       </c>
-      <c r="G2">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="15">
+        <v>-5.71</v>
+      </c>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
         <v>2.9885590415854351E-2</v>
       </c>
-      <c r="H2">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15">
+        <v>-4.6500000000000004</v>
+      </c>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
         <v>0.18840000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="15">
+        <v>-26.26</v>
+      </c>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15">
+        <v>10.52</v>
+      </c>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="15"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>0.12683705033364417</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
+      <c r="B14">
         <v>1.1225128823082477E-11</v>
       </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
+      <c r="C14">
         <v>2.9885590415854351E-2</v>
       </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6">
+      <c r="D14">
         <v>0.18840000000000001</v>
       </c>
-      <c r="F6" s="4" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="F7" s="4" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C8" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="4" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9">
-        <v>80.34</v>
-      </c>
-      <c r="F9" s="4" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10">
-        <v>-5.71</v>
-      </c>
-      <c r="F10" s="4" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
-        <v>-4.6500000000000004</v>
-      </c>
-      <c r="F11" s="4" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>-26.26</v>
-      </c>
-      <c r="F12" s="4" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <v>10.52</v>
-      </c>
-      <c r="F13" s="4" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="4" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="15">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="F15" s="5" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="15">
-        <v>8.01</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15734,10 +15917,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15747,11 +15930,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -16198,461 +16381,461 @@
         <v>7.6838374975171403E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+    <row r="17" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>73.886333333333354</v>
+      </c>
+      <c r="C19">
+        <v>4.6331008115116186</v>
+      </c>
+      <c r="D19">
+        <v>15.947490965392317</v>
+      </c>
+      <c r="E19">
+        <v>1.1105038520767292E-18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>73.886333333333354</v>
+      </c>
+      <c r="I19">
+        <v>4.6331008115116186</v>
+      </c>
+      <c r="J19">
+        <v>15.947490965392317</v>
+      </c>
+      <c r="K19">
+        <v>1.1105038520767292E-18</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" t="s">
-        <v>3</v>
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>7.9648333333333357</v>
+      </c>
+      <c r="C20">
+        <v>5.6743664575390644</v>
+      </c>
+      <c r="D20">
+        <v>1.4036515605634028</v>
+      </c>
+      <c r="E20">
+        <v>0.16833546794509435</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20">
+        <v>7.9648333333333357</v>
+      </c>
+      <c r="I20">
+        <v>5.6743664575390644</v>
+      </c>
+      <c r="J20">
+        <v>1.4036515605634028</v>
+      </c>
+      <c r="K20">
+        <v>0.16833546794509435</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B21">
-        <v>73.886333333333354</v>
+        <v>9.1664999999999992</v>
       </c>
       <c r="C21">
-        <v>4.6331008115116186</v>
+        <v>5.6743664575390635</v>
       </c>
       <c r="D21">
-        <v>15.947490965392317</v>
+        <v>1.6154226323929477</v>
       </c>
       <c r="E21">
-        <v>1.1105038520767292E-18</v>
+        <v>0.11428148205199448</v>
       </c>
       <c r="G21" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="H21">
-        <v>73.886333333333354</v>
+        <v>9.1664999999999992</v>
       </c>
       <c r="I21">
-        <v>4.6331008115116186</v>
+        <v>5.6743664575390635</v>
       </c>
       <c r="J21">
-        <v>15.947490965392317</v>
+        <v>1.6154226323929477</v>
       </c>
       <c r="K21">
-        <v>1.1105038520767292E-18</v>
+        <v>0.11428148205199448</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22">
-        <v>7.9648333333333357</v>
+        <v>1.8291666666666722</v>
       </c>
       <c r="C22">
-        <v>5.6743664575390644</v>
+        <v>5.4327922657912033</v>
       </c>
       <c r="D22">
-        <v>1.4036515605634028</v>
+        <v>0.33668997030945413</v>
       </c>
       <c r="E22">
-        <v>0.16833546794509435</v>
+        <v>0.73815572023050091</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H22">
-        <v>7.9648333333333357</v>
+        <v>1.8291666666666722</v>
       </c>
       <c r="I22">
-        <v>5.6743664575390644</v>
+        <v>5.4327922657912033</v>
       </c>
       <c r="J22">
-        <v>1.4036515605634028</v>
+        <v>0.33668997030945413</v>
       </c>
       <c r="K22">
-        <v>0.16833546794509435</v>
+        <v>0.73815572023050091</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23">
-        <v>9.1664999999999992</v>
+        <v>1.8026666666666635</v>
       </c>
       <c r="C23">
-        <v>5.6743664575390635</v>
+        <v>6.5521940034815236</v>
       </c>
       <c r="D23">
-        <v>1.6154226323929477</v>
+        <v>0.2751241287588268</v>
       </c>
       <c r="E23">
-        <v>0.11428148205199448</v>
+        <v>0.78467324599037991</v>
       </c>
       <c r="G23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H23">
-        <v>9.1664999999999992</v>
+        <v>1.8026666666666635</v>
       </c>
       <c r="I23">
-        <v>5.6743664575390635</v>
+        <v>6.5521940034815236</v>
       </c>
       <c r="J23">
-        <v>1.6154226323929477</v>
+        <v>0.2751241287588268</v>
       </c>
       <c r="K23">
-        <v>0.11428148205199448</v>
+        <v>0.78467324599037991</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24">
-        <v>1.8291666666666722</v>
+        <v>-7.0003333333333275</v>
       </c>
       <c r="C24">
-        <v>5.4327922657912033</v>
+        <v>6.1290162731756412</v>
       </c>
       <c r="D24">
-        <v>0.33668997030945413</v>
+        <v>-1.142162627952402</v>
       </c>
       <c r="E24">
-        <v>0.73815572023050091</v>
+        <v>0.26035041704784678</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H24">
-        <v>1.8291666666666722</v>
+        <v>-7.0003333333333275</v>
       </c>
       <c r="I24">
-        <v>5.4327922657912033</v>
+        <v>6.1290162731756412</v>
       </c>
       <c r="J24">
-        <v>0.33668997030945413</v>
+        <v>-1.142162627952402</v>
       </c>
       <c r="K24">
-        <v>0.73815572023050091</v>
+        <v>0.26035041704784678</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B25">
-        <v>1.8026666666666635</v>
+        <v>6.8969166666666677</v>
       </c>
       <c r="C25">
-        <v>6.5521940034815236</v>
+        <v>6.129016273175643</v>
       </c>
       <c r="D25">
-        <v>0.2751241287588268</v>
+        <v>1.1252893383318021</v>
       </c>
       <c r="E25">
-        <v>0.78467324599037991</v>
+        <v>0.26734417446503389</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H25">
-        <v>1.8026666666666635</v>
+        <v>6.8969166666666677</v>
       </c>
       <c r="I25">
-        <v>6.5521940034815236</v>
+        <v>6.129016273175643</v>
       </c>
       <c r="J25">
-        <v>0.2751241287588268</v>
+        <v>1.1252893383318021</v>
       </c>
       <c r="K25">
-        <v>0.78467324599037991</v>
+        <v>0.26734417446503389</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B26">
-        <v>-7.0003333333333275</v>
+        <v>-25.336333333333325</v>
       </c>
       <c r="C26">
-        <v>6.1290162731756412</v>
+        <v>7.3255755967755904</v>
       </c>
       <c r="D26">
-        <v>-1.142162627952402</v>
+        <v>-3.4586133196803419</v>
       </c>
       <c r="E26">
-        <v>0.26035041704784678</v>
+        <v>1.327912730032603E-3</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H26">
-        <v>-7.0003333333333275</v>
+        <v>-25.336333333333325</v>
       </c>
       <c r="I26">
-        <v>6.1290162731756412</v>
+        <v>7.3255755967755904</v>
       </c>
       <c r="J26">
-        <v>-1.142162627952402</v>
+        <v>-3.4586133196803419</v>
       </c>
       <c r="K26">
-        <v>0.26035041704784678</v>
+        <v>1.327912730032603E-3</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B27">
-        <v>6.8969166666666677</v>
+        <v>9.9916666666660617E-2</v>
       </c>
       <c r="C27">
-        <v>6.129016273175643</v>
+        <v>8.9719611421422822</v>
       </c>
       <c r="D27">
-        <v>1.1252893383318021</v>
+        <v>1.1136546969351117E-2</v>
       </c>
       <c r="E27">
-        <v>0.26734417446503389</v>
+        <v>0.99117127939602578</v>
       </c>
       <c r="G27" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H27">
-        <v>6.8969166666666677</v>
+        <v>9.9916666666660617E-2</v>
       </c>
       <c r="I27">
-        <v>6.129016273175643</v>
+        <v>8.9719611421422822</v>
       </c>
       <c r="J27">
-        <v>1.1252893383318021</v>
+        <v>1.1136546969351117E-2</v>
       </c>
       <c r="K27">
-        <v>0.26734417446503389</v>
+        <v>0.99117127939602578</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B28">
-        <v>-25.336333333333325</v>
+        <v>-2.2165000000000123</v>
       </c>
       <c r="C28">
-        <v>7.3255755967755904</v>
+        <v>9.8282910052222885</v>
       </c>
       <c r="D28">
-        <v>-3.4586133196803419</v>
+        <v>-0.22552242285278989</v>
       </c>
       <c r="E28">
-        <v>1.327912730032603E-3</v>
+        <v>0.82275053376355578</v>
       </c>
       <c r="G28" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H28">
-        <v>-25.336333333333325</v>
+        <v>-2.2165000000000123</v>
       </c>
       <c r="I28">
-        <v>7.3255755967755904</v>
+        <v>9.8282910052222885</v>
       </c>
       <c r="J28">
-        <v>-3.4586133196803419</v>
+        <v>-0.22552242285278989</v>
       </c>
       <c r="K28">
-        <v>1.327912730032603E-3</v>
+        <v>0.82275053376355578</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B29">
-        <v>9.9916666666660617E-2</v>
+        <v>9.6871666666666627</v>
       </c>
       <c r="C29">
-        <v>8.9719611421422822</v>
+        <v>9.1202680677332495</v>
       </c>
       <c r="D29">
-        <v>1.1136546969351117E-2</v>
+        <v>1.0621581070559816</v>
       </c>
       <c r="E29">
-        <v>0.99117127939602578</v>
+        <v>0.29469711104431628</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H29">
-        <v>9.9916666666660617E-2</v>
+        <v>9.6871666666666627</v>
       </c>
       <c r="I29">
-        <v>8.9719611421422822</v>
+        <v>9.1202680677332495</v>
       </c>
       <c r="J29">
-        <v>1.1136546969351117E-2</v>
+        <v>1.0621581070559816</v>
       </c>
       <c r="K29">
-        <v>0.99117127939602578</v>
+        <v>0.29469711104431628</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30">
-        <v>-2.2165000000000123</v>
+        <v>17.139833333333318</v>
       </c>
       <c r="C30">
-        <v>9.8282910052222885</v>
+        <v>9.2662016230232371</v>
       </c>
       <c r="D30">
-        <v>-0.22552242285278989</v>
+        <v>1.8497151293089595</v>
       </c>
       <c r="E30">
-        <v>0.82275053376355578</v>
+        <v>7.1942950271870934E-2</v>
       </c>
       <c r="G30" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H30">
-        <v>-2.2165000000000123</v>
+        <v>17.139833333333318</v>
       </c>
       <c r="I30">
-        <v>9.8282910052222885</v>
+        <v>9.2662016230232371</v>
       </c>
       <c r="J30">
-        <v>-0.22552242285278989</v>
+        <v>1.8497151293089595</v>
       </c>
       <c r="K30">
-        <v>0.82275053376355578</v>
+        <v>7.1942950271870934E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B31">
-        <v>9.6871666666666627</v>
+        <v>1.9597499999999954</v>
       </c>
       <c r="C31">
-        <v>9.1202680677332495</v>
+        <v>9.5513820099986528</v>
       </c>
       <c r="D31">
-        <v>1.0621581070559816</v>
+        <v>0.20517973189099489</v>
       </c>
       <c r="E31">
-        <v>0.29469711104431628</v>
+        <v>0.83849888240737902</v>
       </c>
       <c r="G31" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H31">
-        <v>9.6871666666666627</v>
+        <v>1.9597499999999954</v>
       </c>
       <c r="I31">
-        <v>9.1202680677332495</v>
+        <v>9.5513820099986528</v>
       </c>
       <c r="J31">
-        <v>1.0621581070559816</v>
+        <v>0.20517973189099489</v>
       </c>
       <c r="K31">
-        <v>0.29469711104431628</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32">
-        <v>17.139833333333318</v>
-      </c>
-      <c r="C32">
-        <v>9.2662016230232371</v>
-      </c>
-      <c r="D32">
-        <v>1.8497151293089595</v>
-      </c>
-      <c r="E32">
-        <v>7.1942950271870934E-2</v>
-      </c>
-      <c r="G32" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32">
-        <v>17.139833333333318</v>
-      </c>
-      <c r="I32">
-        <v>9.2662016230232371</v>
-      </c>
-      <c r="J32">
-        <v>1.8497151293089595</v>
-      </c>
-      <c r="K32">
-        <v>7.1942950271870934E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33">
-        <v>1.9597499999999954</v>
-      </c>
-      <c r="C33">
-        <v>9.5513820099986528</v>
-      </c>
-      <c r="D33">
-        <v>0.20517973189099489</v>
-      </c>
-      <c r="E33">
-        <v>0.83849888240737902</v>
-      </c>
-      <c r="G33" t="s">
-        <v>104</v>
-      </c>
-      <c r="H33">
-        <v>1.9597499999999954</v>
-      </c>
-      <c r="I33">
-        <v>9.5513820099986528</v>
-      </c>
-      <c r="J33">
-        <v>0.20517973189099489</v>
-      </c>
-      <c r="K33">
         <v>0.83849888240737902</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16665,7 +16848,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16679,19 +16862,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -16906,11 +17089,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17390,11 +17573,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">

</xml_diff>

<commit_message>
fixed a bug from Common functions
</commit_message>
<xml_diff>
--- a/doc/Supplemental_Tables_drafts.xlsx
+++ b/doc/Supplemental_Tables_drafts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="6030" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="6030" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MLH1.M1_models" sheetId="11" r:id="rId1"/>
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="145">
   <si>
     <t>Estimate</t>
   </si>
@@ -642,6 +642,27 @@
   <si>
     <t xml:space="preserve">           26.356             -0.755             -0.482             -2.649              2.953  </t>
   </si>
+  <si>
+    <t>add M4 M5 (male)</t>
+  </si>
+  <si>
+    <t>strainPERC</t>
+  </si>
+  <si>
+    <t>strainTOM</t>
+  </si>
+  <si>
+    <t>strainAST</t>
+  </si>
+  <si>
+    <t>M4 (male)</t>
+  </si>
+  <si>
+    <t>M5 (male)</t>
+  </si>
+  <si>
+    <t>strainCZECH</t>
+  </si>
 </sst>
 </file>
 
@@ -649,7 +670,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.00000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -736,15 +757,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +794,8 @@
       <xdr:rowOff>204786</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5667374" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1032,7 +1053,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1153,8 +1174,8 @@
       <xdr:rowOff>195261</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6057900" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1508,7 +1529,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1636,8 +1657,8 @@
       <xdr:rowOff>261936</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6029326" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1702,7 +1723,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1714,7 +1735,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1726,7 +1747,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1750,7 +1771,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1762,7 +1783,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2015,7 +2036,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -2196,8 +2217,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5429250" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -2480,7 +2501,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -2597,8 +2618,8 @@
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5457825" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -2881,7 +2902,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -2998,8 +3019,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4267200" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -3254,7 +3275,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -3367,8 +3388,8 @@
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5076825" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -3623,7 +3644,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -4094,8 +4115,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2514600" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -4302,7 +4323,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -4753,8 +4774,8 @@
       <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3133724" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -4985,7 +5006,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -5805,8 +5826,8 @@
       <xdr:rowOff>261936</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6657975" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -6112,7 +6133,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -6233,8 +6254,8 @@
       <xdr:rowOff>244608</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4876800" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -6517,7 +6538,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -6634,8 +6655,8 @@
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4524375" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -6890,7 +6911,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -7008,8 +7029,8 @@
       <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4838700" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -7339,7 +7360,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -7460,8 +7481,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4514850" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -7768,7 +7789,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -7885,8 +7906,8 @@
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3581400" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -8165,7 +8186,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -8283,8 +8304,8 @@
       <xdr:rowOff>204786</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7200900" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -8593,7 +8614,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -8722,8 +8743,8 @@
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4667250" cy="344453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -9006,7 +9027,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -9123,8 +9144,8 @@
       <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4429124" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -9379,7 +9400,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -9492,11 +9513,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9516,19 +9537,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_male_glm" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_female_glm" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_female_glm" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9832,12 +9853,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -9851,7 +9872,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B4">
@@ -9866,7 +9887,7 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B5">
@@ -9881,7 +9902,7 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B6">
@@ -9896,7 +9917,7 @@
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B7">
@@ -9912,7 +9933,7 @@
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="21"/>
       <c r="D8" t="s">
         <v>29</v>
       </c>
@@ -9922,7 +9943,7 @@
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="21"/>
       <c r="D9" t="s">
         <v>30</v>
       </c>
@@ -10045,8 +10066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10064,19 +10085,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -10476,16 +10497,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -11460,16 +11481,16 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -12474,11 +12495,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -13022,11 +13043,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -13595,11 +13616,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -13763,11 +13784,11 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -13927,11 +13948,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -14161,11 +14182,11 @@
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -14420,12 +14441,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -14653,15 +14674,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -14670,11 +14691,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -14722,7 +14743,7 @@
       <c r="E3" s="6">
         <v>6.8476448906856882E-83</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
         <v>4</v>
@@ -14756,7 +14777,7 @@
       <c r="E4" s="6">
         <v>3.1331650862026381E-4</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
       <c r="H4" t="s">
         <v>105</v>
       </c>
@@ -14789,7 +14810,7 @@
       <c r="E5" s="6">
         <v>2.9994818416794007E-3</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
       <c r="H5" t="s">
         <v>106</v>
       </c>
@@ -14822,7 +14843,7 @@
       <c r="E6" s="6">
         <v>7.8263498735992003E-13</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
         <v>92</v>
@@ -14856,7 +14877,7 @@
       <c r="E7" s="6">
         <v>5.9726584202964396E-5</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
       <c r="H7" t="s">
         <v>93</v>
       </c>
@@ -14889,7 +14910,7 @@
       <c r="E8" s="6">
         <v>0.66364908711553217</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="19"/>
       <c r="H8" t="s">
         <v>94</v>
       </c>
@@ -14922,7 +14943,7 @@
       <c r="E9" s="6">
         <v>0.58049315316905858</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="19"/>
       <c r="H9" t="s">
         <v>96</v>
       </c>
@@ -14940,22 +14961,22 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="17">
         <v>-345.00471099408134</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="17">
         <v>58.199900153131743</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="17">
         <v>-5.9279261663048848</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="17">
         <v>2.5617511159882357E-8</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
       <c r="H10" t="s">
         <v>98</v>
       </c>
@@ -14988,7 +15009,7 @@
       <c r="E11" s="6">
         <v>0.34616907888281573</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="20"/>
       <c r="H11" t="s">
         <v>107</v>
       </c>
@@ -15021,7 +15042,7 @@
       <c r="E12" s="6">
         <v>1.3470832207404887E-2</v>
       </c>
-      <c r="F12" s="20"/>
+      <c r="F12" s="19"/>
       <c r="H12" t="s">
         <v>108</v>
       </c>
@@ -15054,7 +15075,7 @@
       <c r="E13" s="6">
         <v>4.3552294070361525E-4</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="19"/>
       <c r="H13" t="s">
         <v>99</v>
       </c>
@@ -15087,7 +15108,7 @@
       <c r="E14" s="6">
         <v>7.3796863466524351E-2</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="20"/>
       <c r="H14" t="s">
         <v>100</v>
       </c>
@@ -15120,7 +15141,7 @@
       <c r="E15" s="6">
         <v>0.19381122451147587</v>
       </c>
-      <c r="F15" s="20"/>
+      <c r="F15" s="19"/>
       <c r="H15" t="s">
         <v>101</v>
       </c>
@@ -15153,7 +15174,7 @@
       <c r="E16" s="6">
         <v>0.32588118321571224</v>
       </c>
-      <c r="F16" s="20"/>
+      <c r="F16" s="19"/>
       <c r="H16" t="s">
         <v>103</v>
       </c>
@@ -15175,14 +15196,14 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="19" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -15461,7 +15482,7 @@
       <c r="E28" s="6">
         <v>2.5617511159882205E-8</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="2"/>
       <c r="H28" t="s">
         <v>98</v>
@@ -15675,6 +15696,455 @@
       </c>
       <c r="L34">
         <v>0.34616907888281784</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>1338.3786022420861</v>
+      </c>
+      <c r="C38">
+        <v>23.386706046603653</v>
+      </c>
+      <c r="D38">
+        <v>57.228179102052422</v>
+      </c>
+      <c r="E38">
+        <v>4.9396824791406674E-56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39">
+        <v>236.87871396784379</v>
+      </c>
+      <c r="C39">
+        <v>41.835411592008917</v>
+      </c>
+      <c r="D39">
+        <v>5.6621580845900068</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3.9497517062357979E-7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40">
+        <v>213.99626455778031</v>
+      </c>
+      <c r="C40">
+        <v>37.502160613536581</v>
+      </c>
+      <c r="D40">
+        <v>5.7062382821894628</v>
+      </c>
+      <c r="E40" s="2">
+        <v>3.331143813140082E-7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41">
+        <v>127.96729625070191</v>
+      </c>
+      <c r="C41">
+        <v>33.073796870339748</v>
+      </c>
+      <c r="D41">
+        <v>3.8691444091640323</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2.6162844142097618E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42">
+        <v>78.835972072487849</v>
+      </c>
+      <c r="C42">
+        <v>37.502160613536581</v>
+      </c>
+      <c r="D42">
+        <v>2.1021714691294782</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3.9541462868423451E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43">
+        <v>109.97854061505643</v>
+      </c>
+      <c r="C43">
+        <v>81.013926188791615</v>
+      </c>
+      <c r="D43">
+        <v>1.3575263635386197</v>
+      </c>
+      <c r="E43">
+        <v>0.17945709000962828</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44">
+        <v>3.0933805932666241</v>
+      </c>
+      <c r="C44">
+        <v>44.218812969867663</v>
+      </c>
+      <c r="D44">
+        <v>6.9956210615028686E-2</v>
+      </c>
+      <c r="E44">
+        <v>0.94445009835469795</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45">
+        <v>190.26599858474856</v>
+      </c>
+      <c r="C45">
+        <v>45.41737194439802</v>
+      </c>
+      <c r="D45">
+        <v>4.1892780325924779</v>
+      </c>
+      <c r="E45" s="2">
+        <v>8.8755130112118128E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46">
+        <v>-161.33860138707749</v>
+      </c>
+      <c r="C46">
+        <v>49.056368462464597</v>
+      </c>
+      <c r="D46">
+        <v>-3.288841111639266</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1.6489175335300582E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47">
+        <v>-91.64834772852511</v>
+      </c>
+      <c r="C47">
+        <v>41.835411592008917</v>
+      </c>
+      <c r="D47">
+        <v>-2.1906883245779056</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3.2182052386035574E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48">
+        <v>72.492683790069762</v>
+      </c>
+      <c r="C48">
+        <v>64.895475587816662</v>
+      </c>
+      <c r="D48">
+        <v>1.1170683800902661</v>
+      </c>
+      <c r="E48">
+        <v>0.26820722175796674</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49">
+        <v>39.557007397496776</v>
+      </c>
+      <c r="C49">
+        <v>64.895475587816662</v>
+      </c>
+      <c r="D49">
+        <v>0.60954954161585839</v>
+      </c>
+      <c r="E49">
+        <v>0.54435243368619524</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>1338.3786022420861</v>
+      </c>
+      <c r="C53">
+        <v>23.386706046603653</v>
+      </c>
+      <c r="D53">
+        <v>57.228179102052422</v>
+      </c>
+      <c r="E53">
+        <v>4.9396824791406674E-56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54">
+        <v>127.96729625070195</v>
+      </c>
+      <c r="C54">
+        <v>33.073796870339756</v>
+      </c>
+      <c r="D54">
+        <v>3.8691444091640328</v>
+      </c>
+      <c r="E54" s="2">
+        <v>2.6162844142097613E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55">
+        <v>78.835972072487834</v>
+      </c>
+      <c r="C55">
+        <v>37.502160613536581</v>
+      </c>
+      <c r="D55">
+        <v>2.1021714691294777</v>
+      </c>
+      <c r="E55" s="2">
+        <v>3.9541462868423485E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56">
+        <v>109.9785406150564</v>
+      </c>
+      <c r="C56">
+        <v>81.013926188791601</v>
+      </c>
+      <c r="D56">
+        <v>1.3575263635386197</v>
+      </c>
+      <c r="E56">
+        <v>0.17945709000962828</v>
+      </c>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57">
+        <v>239.9720945611104</v>
+      </c>
+      <c r="C57">
+        <v>36.041334559250707</v>
+      </c>
+      <c r="D57">
+        <v>6.6582466353071519</v>
+      </c>
+      <c r="E57" s="2">
+        <v>7.8476194379247186E-9</v>
+      </c>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58">
+        <v>404.26226314252892</v>
+      </c>
+      <c r="C58">
+        <v>41.835411592008903</v>
+      </c>
+      <c r="D58">
+        <v>9.6631596955472094</v>
+      </c>
+      <c r="E58" s="2">
+        <v>4.6873235494355556E-14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59">
+        <v>213.99626455778039</v>
+      </c>
+      <c r="C59">
+        <v>37.502160613536589</v>
+      </c>
+      <c r="D59">
+        <v>5.7062382821894637</v>
+      </c>
+      <c r="E59" s="2">
+        <v>3.331143813140082E-7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60">
+        <v>75.540112580766305</v>
+      </c>
+      <c r="C60">
+        <v>41.835411592008903</v>
+      </c>
+      <c r="D60">
+        <v>1.8056500391930035</v>
+      </c>
+      <c r="E60">
+        <v>7.5750955551022292E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61">
+        <v>145.2303662393187</v>
+      </c>
+      <c r="C61">
+        <v>33.073796870339763</v>
+      </c>
+      <c r="D61">
+        <v>4.3911005080145422</v>
+      </c>
+      <c r="E61" s="2">
+        <v>4.3967746987810889E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62">
+        <v>309.3713977579136</v>
+      </c>
+      <c r="C62">
+        <v>59.624635245145214</v>
+      </c>
+      <c r="D62">
+        <v>5.1886505717970559</v>
+      </c>
+      <c r="E62" s="2">
+        <v>2.4010311086635611E-6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63">
+        <v>276.43572136534056</v>
+      </c>
+      <c r="C63">
+        <v>59.624635245145207</v>
+      </c>
+      <c r="D63">
+        <v>4.6362668757432557</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1.8367392490764613E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64">
+        <v>236.87871396784379</v>
+      </c>
+      <c r="C64">
+        <v>41.83541159200891</v>
+      </c>
+      <c r="D64">
+        <v>5.6621580845900086</v>
+      </c>
+      <c r="E64" s="2">
+        <v>3.9497517062357539E-7</v>
       </c>
     </row>
   </sheetData>
@@ -15683,7 +16153,8 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15706,13 +16177,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -15729,7 +16200,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B3">
@@ -15744,7 +16215,7 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B4">
@@ -15759,7 +16230,7 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B5">
@@ -15774,7 +16245,7 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>53</v>
       </c>
       <c r="B6">
@@ -15930,11 +16401,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -16382,11 +16853,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -16862,13 +17333,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17089,11 +17560,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17573,11 +18044,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">

</xml_diff>

<commit_message>
finalizing the v3 draft
</commit_message>
<xml_diff>
--- a/doc/Supplemental_Tables_drafts.xlsx
+++ b/doc/Supplemental_Tables_drafts.xlsx
@@ -12,44 +12,44 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="6030" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="MLH1.M1_models" sheetId="11" r:id="rId1"/>
-    <sheet name="MLH1_M2.M3" sheetId="1" r:id="rId2"/>
-    <sheet name="MLH1_M4.M5" sheetId="3" r:id="rId3"/>
-    <sheet name="Total.SC.M1" sheetId="5" r:id="rId4"/>
-    <sheet name="Total.SC_M2_M3" sheetId="13" r:id="rId5"/>
-    <sheet name="Total.SC_M4_M5" sheetId="21" r:id="rId6"/>
-    <sheet name="Short.bivalent_M1.SC" sheetId="6" r:id="rId7"/>
-    <sheet name="Short.bivalent_M2_M3" sheetId="15" r:id="rId8"/>
-    <sheet name="Short.bivalent_M4_M5" sheetId="24" r:id="rId9"/>
-    <sheet name="Normalized.Foci.Pos_M1" sheetId="7" r:id="rId10"/>
-    <sheet name="Normalized.Foci.Pos_M2" sheetId="18" r:id="rId11"/>
-    <sheet name="Nrm.Pos_M4.M5" sheetId="23" r:id="rId12"/>
-    <sheet name="IFD_M1" sheetId="20" r:id="rId13"/>
-    <sheet name="IFD_M2_M3" sheetId="8" r:id="rId14"/>
-    <sheet name="IFD_M4_M5" sheetId="22" r:id="rId15"/>
+    <sheet name="1.MLH1.M1_models" sheetId="11" r:id="rId1"/>
+    <sheet name="2.MLH1_M2.M3" sheetId="1" r:id="rId2"/>
+    <sheet name="3.MLH1_M4.M5" sheetId="3" r:id="rId3"/>
+    <sheet name="4.Total.SC.M1" sheetId="5" r:id="rId4"/>
+    <sheet name="5.Total.SC_M2_M3" sheetId="13" r:id="rId5"/>
+    <sheet name="6.Total.SC_M4_M5" sheetId="21" r:id="rId6"/>
+    <sheet name="7.Short.bivalent_M1.SC" sheetId="6" r:id="rId7"/>
+    <sheet name="8.Short.bivalent_M2_M3" sheetId="15" r:id="rId8"/>
+    <sheet name="9.Short.bivalent_M4_M5" sheetId="24" r:id="rId9"/>
+    <sheet name="10.Normalized.Foci.Pos_M1" sheetId="7" r:id="rId10"/>
+    <sheet name="11.Normalized.Foci.Pos_M2" sheetId="18" r:id="rId11"/>
+    <sheet name="12.Nrm.Pos_M4.M5" sheetId="23" r:id="rId12"/>
+    <sheet name="13.IFD_M1" sheetId="20" r:id="rId13"/>
+    <sheet name="14.IFD_M2_M3" sheetId="8" r:id="rId14"/>
+    <sheet name="15.IFD_M4_M5" sheetId="22" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="ABS.IFD_Q1_M1" localSheetId="12">IFD_M1!#REF!</definedName>
-    <definedName name="ABS.IFD_Q1_M1" localSheetId="13">IFD_M2_M3!#REF!</definedName>
-    <definedName name="ABS.IFD_Q1_M2" localSheetId="13">IFD_M2_M3!$A$3:$E$17</definedName>
-    <definedName name="ABS.IFD_Q1_M3" localSheetId="13">IFD_M2_M3!$A$21:$E$36</definedName>
-    <definedName name="MLH1_M1_glm" localSheetId="0">'MLH1.M1_models'!#REF!</definedName>
-    <definedName name="MLH1_M2_glm" localSheetId="1">MLH1_M2.M3!$A$2:$E$18</definedName>
-    <definedName name="MLH1_M4_female_glm" localSheetId="2">MLH1_M4.M5!$A$2:$E$10</definedName>
-    <definedName name="MLH1_M4_male_glm" localSheetId="2">MLH1_M4.M5!$A$25:$E$37</definedName>
-    <definedName name="MLH1_M5_female_glm" localSheetId="2">MLH1_M4.M5!$A$13:$E$21</definedName>
-    <definedName name="MLH1_M5_male_glm" localSheetId="2">MLH1_M4.M5!$A$40:$E$52</definedName>
-    <definedName name="Nrm1CO_Pos_Q1_M1" localSheetId="9">Normalized.Foci.Pos_M1!#REF!</definedName>
-    <definedName name="Nrm1CO_Pos_Q1_M2" localSheetId="10">Normalized.Foci.Pos_M2!$A$2:$E$16</definedName>
-    <definedName name="Nrm1CO_Pos_Q1_M3" localSheetId="10">Normalized.Foci.Pos_M2!$A$19:$E$33</definedName>
-    <definedName name="PER.IFD_Q1_M2" localSheetId="13">IFD_M2_M3!$M$2:$Q$17</definedName>
-    <definedName name="PER.IFD_Q1_M3" localSheetId="13">IFD_M2_M3!$M$21:$Q$36</definedName>
-    <definedName name="ShortSC_Q1_M1" localSheetId="6">Short.bivalent_M1.SC!#REF!</definedName>
-    <definedName name="ShortSC_Q1_M1" localSheetId="3">Total.SC.M1!#REF!</definedName>
-    <definedName name="ShortSC_Q1_M2" localSheetId="7">Short.bivalent_M2_M3!$A$2:$E$15</definedName>
-    <definedName name="ShortSC_Q1_M3" localSheetId="7">Short.bivalent_M2_M3!$A$18:$E$31</definedName>
-    <definedName name="ShortSC_Q1_M3" localSheetId="4">Total.SC_M2_M3!$A$20:$E$34</definedName>
-    <definedName name="TotalSC_Q1_M2" localSheetId="4">Total.SC_M2_M3!$A$2:$E$17</definedName>
+    <definedName name="ABS.IFD_Q1_M1" localSheetId="12">'13.IFD_M1'!#REF!</definedName>
+    <definedName name="ABS.IFD_Q1_M1" localSheetId="13">'14.IFD_M2_M3'!#REF!</definedName>
+    <definedName name="ABS.IFD_Q1_M2" localSheetId="13">'14.IFD_M2_M3'!$A$3:$E$17</definedName>
+    <definedName name="ABS.IFD_Q1_M3" localSheetId="13">'14.IFD_M2_M3'!$A$21:$E$36</definedName>
+    <definedName name="MLH1_M1_glm" localSheetId="0">'1.MLH1.M1_models'!#REF!</definedName>
+    <definedName name="MLH1_M2_glm" localSheetId="1">'2.MLH1_M2.M3'!$A$2:$E$18</definedName>
+    <definedName name="MLH1_M4_female_glm" localSheetId="2">'3.MLH1_M4.M5'!$A$2:$E$10</definedName>
+    <definedName name="MLH1_M4_male_glm" localSheetId="2">'3.MLH1_M4.M5'!$A$25:$E$37</definedName>
+    <definedName name="MLH1_M5_female_glm" localSheetId="2">'3.MLH1_M4.M5'!$A$13:$E$21</definedName>
+    <definedName name="MLH1_M5_male_glm" localSheetId="2">'3.MLH1_M4.M5'!$A$40:$E$52</definedName>
+    <definedName name="Nrm1CO_Pos_Q1_M1" localSheetId="9">'10.Normalized.Foci.Pos_M1'!#REF!</definedName>
+    <definedName name="Nrm1CO_Pos_Q1_M2" localSheetId="10">'11.Normalized.Foci.Pos_M2'!$A$2:$E$16</definedName>
+    <definedName name="Nrm1CO_Pos_Q1_M3" localSheetId="10">'11.Normalized.Foci.Pos_M2'!$A$19:$E$33</definedName>
+    <definedName name="PER.IFD_Q1_M2" localSheetId="13">'14.IFD_M2_M3'!$N$2:$R$17</definedName>
+    <definedName name="PER.IFD_Q1_M3" localSheetId="13">'14.IFD_M2_M3'!$N$21:$R$36</definedName>
+    <definedName name="ShortSC_Q1_M1" localSheetId="3">'4.Total.SC.M1'!#REF!</definedName>
+    <definedName name="ShortSC_Q1_M1" localSheetId="6">'7.Short.bivalent_M1.SC'!#REF!</definedName>
+    <definedName name="ShortSC_Q1_M2" localSheetId="7">'8.Short.bivalent_M2_M3'!$A$2:$E$15</definedName>
+    <definedName name="ShortSC_Q1_M3" localSheetId="4">'5.Total.SC_M2_M3'!$A$20:$E$34</definedName>
+    <definedName name="ShortSC_Q1_M3" localSheetId="7">'8.Short.bivalent_M2_M3'!$A$18:$E$31</definedName>
+    <definedName name="TotalSC_Q1_M2" localSheetId="4">'5.Total.SC_M2_M3'!$A$2:$E$17</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="165">
   <si>
     <t>Estimate</t>
   </si>
@@ -647,9 +647,6 @@
     <t xml:space="preserve">           26.356             -0.755             -0.482             -2.649              2.953  </t>
   </si>
   <si>
-    <t>add M4 M5 (male)</t>
-  </si>
-  <si>
     <t>strainPERC</t>
   </si>
   <si>
@@ -718,6 +715,18 @@
   <si>
     <t>M5.male_shortBiv</t>
   </si>
+  <si>
+    <t>M5 total SC female</t>
+  </si>
+  <si>
+    <t>M4 (female</t>
+  </si>
+  <si>
+    <t>M4 Long male</t>
+  </si>
+  <si>
+    <t>M5 long male</t>
+  </si>
 </sst>
 </file>
 
@@ -776,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -810,6 +819,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2667,7 +2679,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
@@ -3437,7 +3449,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
@@ -9908,12 +9920,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -9927,7 +9939,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B4">
@@ -9942,7 +9954,7 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B5">
@@ -9957,7 +9969,7 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B6">
@@ -9972,7 +9984,7 @@
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B7">
@@ -9988,7 +10000,7 @@
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="D8" t="s">
         <v>29</v>
       </c>
@@ -9998,7 +10010,7 @@
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="D9" t="s">
         <v>30</v>
       </c>
@@ -10136,13 +10148,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -10354,7 +10366,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10363,11 +10375,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -10847,11 +10859,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -11345,7 +11357,7 @@
   <dimension ref="A2:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11356,7 +11368,7 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -11371,7 +11383,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -11646,7 +11658,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -11661,7 +11673,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -11919,7 +11931,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23">
         <v>-4.188162354509304E-2</v>
@@ -11968,19 +11980,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -12354,10 +12366,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView topLeftCell="I19" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12367,31 +12379,33 @@
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" customWidth="1"/>
-    <col min="13" max="13" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.28515625" customWidth="1"/>
-    <col min="19" max="19" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
+    <col min="14" max="14" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="20" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="17"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -12408,47 +12422,48 @@
         <v>3</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="H2" t="s">
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>118</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>119</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>120</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>118</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>119</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -12465,53 +12480,54 @@
         <v>1.04037532975528E-21</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>53.713237564634042</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>3.8726264967669741</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>13.869976257580232</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>8.1835314282680017E-21</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="6">
+      <c r="O3" s="6">
         <v>0.46085531896958898</v>
       </c>
-      <c r="O3" s="6">
+      <c r="P3" s="6">
         <v>2.3261536212087399E-2</v>
       </c>
-      <c r="P3" s="6">
+      <c r="Q3" s="6">
         <v>19.811903855692702</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="R3" s="6">
         <v>1.7522479931949099E-29</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>4</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.4608553189695892</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>2.3431856144382271E-2</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>19.66789639411806</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>1.3821289710965012E-28</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -12528,53 +12544,54 @@
         <v>9.0467702926530794E-2</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" t="s">
         <v>105</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>8.7318604745816533</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5.1956736589426944</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.6806021793829451</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>9.7792419393728611E-2</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="6">
+      <c r="O4" s="6">
         <v>2.0578482236366501E-2</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="6">
         <v>3.12086257387802E-2</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <v>0.65938444097509197</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="R4" s="6">
         <v>0.51194319301494495</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>105</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>2.057848223636647E-2</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>3.1437133906700929E-2</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0.65459155078956155</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>0.51511354277405197</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -12591,53 +12608,54 @@
         <v>0.61027406389588801</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" t="s">
         <v>106</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>6.6802137047705319</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>5.4767209137332609</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1.219746963556136</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.2271074805715195</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <v>2.9519099825737198E-3</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <v>4.8422749028052603E-2</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <v>6.0961222603524698E-2</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="R5" s="6">
         <v>0.95157431831941297</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>106</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>1.1732287972722971E-2</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>3.3137648750960744E-2</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>0.35404708586582573</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>0.72448582066622014</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -12654,53 +12672,54 @@
         <v>0.26044980027197701</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" t="s">
         <v>98</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>-5.7687760261724987</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5.1956736589426944</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>-1.1103037651803616</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.27108804371015555</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="6">
+      <c r="O6" s="6">
         <v>8.1742163352924904E-2</v>
       </c>
-      <c r="O6" s="6">
+      <c r="P6" s="6">
         <v>3.12086257387802E-2</v>
       </c>
-      <c r="P6" s="6">
+      <c r="Q6" s="6">
         <v>2.6192170086922801</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="6">
         <v>1.09227982377413E-2</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>98</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>8.1742163352924863E-2</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>3.1437133906700929E-2</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>2.6001786166486776</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>1.1594484373726614E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -12717,53 +12736,54 @@
         <v>0.18611096316811199</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" t="s">
         <v>92</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>6.5340266375720288</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>4.999539309353354</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1.3069257452077414</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.19598838709284738</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <v>2.6801241819794999E-2</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>3.0030514118871698E-2</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>0.89246696589028995</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>0.37538516802156602</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>92</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>2.6801241819794951E-2</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>3.0250396205973491E-2</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>0.88597986080270108</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>0.37899780119980925</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -12780,53 +12800,54 @@
         <v>0.44914915404691902</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" t="s">
         <v>93</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>3.5323492828638061</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>4.7429794407305268</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.74475323517736858</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.45919016169480131</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <v>1.22967068285169E-2</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>2.8489447176443802E-2</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>0.43162321656716102</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>0.66742199647298095</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>93</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>1.2296706828516862E-2</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>2.8698045640017673E-2</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>0.42848586216511741</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>0.66975890610550015</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -12843,53 +12864,54 @@
         <v>0.106392545994445</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" t="s">
         <v>94</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>-6.9176240307994075</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>4.3200957167221619</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-1.6012663802847635</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.11432088013963991</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="6">
         <v>-1.89314347652747E-3</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <v>2.5949330005904499E-2</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <v>-7.2955389449234298E-2</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>0.942062265640912</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>94</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>-1.8931434765274739E-3</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>2.6139329844668692E-2</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>-7.2425096120572283E-2</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>0.94249305867159439</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -12906,23 +12928,24 @@
         <v>0.64949157240539501</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="M10" t="s">
+      <c r="G10" s="6"/>
+      <c r="N10" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="6">
         <v>8.7803779901492601E-3</v>
       </c>
-      <c r="O10" s="6">
+      <c r="P10" s="6">
         <v>3.5532583490948899E-2</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <v>0.24710778467278799</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>0.80559186620130796</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -12939,53 +12962,54 @@
         <v>5.1651703417117202E-2</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" t="s">
         <v>96</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>-10.072847607037563</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>5.1956736589426953</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>-1.9386990539138977</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>5.7020704710277183E-2</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>43</v>
       </c>
-      <c r="N11" s="6">
+      <c r="O11" s="6">
         <v>3.0934248967801899E-4</v>
       </c>
-      <c r="O11" s="6">
+      <c r="P11" s="6">
         <v>3.12086257387802E-2</v>
       </c>
-      <c r="P11" s="6">
+      <c r="Q11" s="6">
         <v>9.91208303330148E-3</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="R11" s="6">
         <v>0.99212133233197997</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>96</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>3.0934248967801487E-4</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>3.1437133906700936E-2</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>9.8400347371385994E-3</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>0.99218000897018643</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -13002,53 +13026,54 @@
         <v>0.25373448308222801</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" t="s">
         <v>107</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>-8.6500413492625228</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>7.6804380214682952</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>-1.1262432331442556</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.26433447425299872</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="6">
+      <c r="O12" s="6">
         <v>-4.3075505327091597E-2</v>
       </c>
-      <c r="O12" s="6">
+      <c r="P12" s="6">
         <v>4.6133751166095999E-2</v>
       </c>
-      <c r="P12" s="6">
+      <c r="Q12" s="6">
         <v>-0.93370914435304098</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="R12" s="6">
         <v>0.35385743446773898</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>107</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>-4.3075505327091645E-2</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>4.6471540437770791E-2</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>-0.92692226083560292</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>0.35750438799522793</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -13065,53 +13090,54 @@
         <v>0.61082491583855203</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" t="s">
         <v>108</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>-3.9380085765654056</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>7.8732823776559755</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>-0.50017367441834659</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.61869550092109316</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="6">
+      <c r="O13" s="6">
         <v>-1.5983525492887701E-2</v>
       </c>
-      <c r="O13" s="6">
+      <c r="P13" s="6">
         <v>4.7292100926523799E-2</v>
       </c>
-      <c r="P13" s="6">
+      <c r="Q13" s="6">
         <v>-0.33797452808706502</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="R13" s="6">
         <v>0.736455073633836</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>108</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>-1.5983525492887722E-2</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>4.7638371583562447E-2</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>-0.33551788110244335</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>0.73834921608549242</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -13128,53 +13154,54 @@
         <v>0.67557115913499199</v>
       </c>
       <c r="F14" s="6"/>
-      <c r="G14" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" t="s">
         <v>124</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>-2.7170521218343566</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>6.6074670114508001</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>-0.41120933591127745</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.6823145344035032</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>63</v>
       </c>
-      <c r="N14" s="6">
+      <c r="O14" s="6">
         <v>-2.93493724345451E-2</v>
       </c>
-      <c r="O14" s="6">
+      <c r="P14" s="6">
         <v>3.9688783125703099E-2</v>
       </c>
-      <c r="P14" s="6">
+      <c r="Q14" s="6">
         <v>-0.73948783820328401</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="R14" s="6">
         <v>0.462232965617632</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>124</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>-2.9349372434545124E-2</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>3.9979382628384373E-2</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>-0.7341126977210447</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>0.4656035503041151</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -13191,53 +13218,54 @@
         <v>0.95515878597181803</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" t="s">
         <v>125</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.37646142367103663</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>6.8184625502184231</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>5.5212068834927755E-2</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.95614423789298542</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>64</v>
       </c>
-      <c r="N15" s="6">
+      <c r="O15" s="6">
         <v>-2.67907261490406E-4</v>
       </c>
-      <c r="O15" s="6">
+      <c r="P15" s="6">
         <v>4.09561608007072E-2</v>
       </c>
-      <c r="P15" s="6">
+      <c r="Q15" s="6">
         <v>-6.5413177468963404E-3</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="R15" s="6">
         <v>0.99480055281438395</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>125</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>-2.6790726149041115E-4</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>4.125603998628781E-2</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>-6.4937706473877513E-3</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>0.99483927653687187</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -13254,53 +13282,54 @@
         <v>9.4629519978275903E-3</v>
       </c>
       <c r="F16" s="6"/>
-      <c r="G16" t="s">
+      <c r="G16" s="6"/>
+      <c r="H16" t="s">
         <v>126</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>18.609694944960697</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>7.1173963240096452</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>2.6146773479767065</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>1.1160621567181114E-2</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>58</v>
       </c>
-      <c r="N16" s="6">
+      <c r="O16" s="6">
         <v>8.5207167240391804E-2</v>
       </c>
-      <c r="O16" s="6">
+      <c r="P16" s="6">
         <v>4.2751753226123297E-2</v>
       </c>
-      <c r="P16" s="6">
+      <c r="Q16" s="6">
         <v>1.9930683728855001</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="R16" s="6">
         <v>5.0390944266193803E-2</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>126</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>8.5207167240391957E-2</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>4.3064779659484007E-2</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>1.9785812887963325</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>5.2239032252814545E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -13317,65 +13346,67 @@
         <v>3.8026406271824799E-3</v>
       </c>
       <c r="F17" s="6"/>
-      <c r="G17" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" t="s">
         <v>127</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>21.876220481084694</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>7.4539377880589495</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>2.9348541808505479</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>4.651637775698025E-3</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>60</v>
       </c>
-      <c r="N17" s="6">
+      <c r="O17" s="6">
         <v>0.120858551679667</v>
       </c>
-      <c r="O17" s="6">
+      <c r="P17" s="6">
         <v>4.4773242119872103E-2</v>
       </c>
-      <c r="P17" s="6">
+      <c r="Q17" s="6">
         <v>2.6993477791063301</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="R17" s="6">
         <v>8.81511325827764E-3</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>127</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>0.12085855167966691</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>4.5101069804894742E-2</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>2.6797269377976116</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>9.3901481158108497E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="17"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -13392,47 +13423,48 @@
         <v>3</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="H21" t="s">
+      <c r="G21" s="2"/>
+      <c r="I21" t="s">
         <v>0</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>118</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>119</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>120</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>0</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>1</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>2</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>3</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>0</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>118</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>119</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -13449,53 +13481,54 @@
         <v>1.04037532975528E-21</v>
       </c>
       <c r="F22" s="6"/>
-      <c r="G22" t="s">
+      <c r="G22" s="6"/>
+      <c r="H22" t="s">
         <v>4</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>53.713237564634035</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>3.8726264967669737</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>13.869976257580232</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>8.1835314282680017E-21</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>4</v>
       </c>
-      <c r="N22" s="6">
+      <c r="O22" s="6">
         <v>0.46085531896958898</v>
       </c>
-      <c r="O22" s="6">
+      <c r="P22" s="6">
         <v>2.3261536212087399E-2</v>
       </c>
-      <c r="P22" s="6">
+      <c r="Q22" s="6">
         <v>19.811903855692702</v>
       </c>
-      <c r="Q22" s="6">
+      <c r="R22" s="6">
         <v>1.75224799319486E-29</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>4</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>0.46085531896958931</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>2.3431856144382267E-2</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>19.66789639411807</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>1.3821289710964817E-28</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -13512,53 +13545,54 @@
         <v>0.26044980027197701</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" t="s">
+      <c r="G23" s="6"/>
+      <c r="H23" t="s">
         <v>98</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>-5.768776026172497</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>5.1956736589426926</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>-1.1103037651803616</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>0.27108804371015555</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>36</v>
       </c>
-      <c r="N23" s="6">
+      <c r="O23" s="6">
         <v>8.1742163352924793E-2</v>
       </c>
-      <c r="O23" s="6">
+      <c r="P23" s="6">
         <v>3.12086257387802E-2</v>
       </c>
-      <c r="P23" s="6">
+      <c r="Q23" s="6">
         <v>2.6192170086922801</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="R23" s="6">
         <v>1.09227982377413E-2</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>98</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>8.1742163352924835E-2</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>3.1437133906700922E-2</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>2.6001786166486776</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>1.1594484373726614E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -13575,53 +13609,54 @@
         <v>0.18611096316811199</v>
       </c>
       <c r="F24" s="6"/>
-      <c r="G24" t="s">
+      <c r="G24" s="6"/>
+      <c r="H24" t="s">
         <v>92</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>6.534026637572028</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>4.9995393093533522</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1.3069257452077416</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>0.19598838709284727</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="6">
+      <c r="O24" s="6">
         <v>2.6801241819794999E-2</v>
       </c>
-      <c r="O24" s="6">
+      <c r="P24" s="6">
         <v>3.0030514118871698E-2</v>
       </c>
-      <c r="P24" s="6">
+      <c r="Q24" s="6">
         <v>0.89246696589028995</v>
       </c>
-      <c r="Q24" s="6">
+      <c r="R24" s="6">
         <v>0.37538516802156602</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>92</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>2.6801241819794961E-2</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>3.0250396205973477E-2</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>0.88597986080270186</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>0.37899780119980886</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -13638,53 +13673,54 @@
         <v>0.44914915404691902</v>
       </c>
       <c r="F25" s="6"/>
-      <c r="G25" t="s">
+      <c r="G25" s="6"/>
+      <c r="H25" t="s">
         <v>93</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>3.5323492828638074</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>4.7429794407305277</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>0.74475323517736869</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>0.45919016169480131</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="6">
+      <c r="O25" s="6">
         <v>1.22967068285169E-2</v>
       </c>
-      <c r="O25" s="6">
+      <c r="P25" s="6">
         <v>2.8489447176443802E-2</v>
       </c>
-      <c r="P25" s="6">
+      <c r="Q25" s="6">
         <v>0.43162321656716102</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="R25" s="6">
         <v>0.66742199647298095</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>93</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>1.2296706828516869E-2</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>2.8698045640017683E-2</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>0.42848586216511753</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>0.66975890610550004</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -13701,53 +13737,54 @@
         <v>0.69155343838387096</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" t="s">
+      <c r="G26" s="6"/>
+      <c r="H26" t="s">
         <v>94</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>1.8142364437822482</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>4.6543178016046012</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>0.389796425838558</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>0.69800177513725425</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>40</v>
       </c>
-      <c r="N26" s="6">
+      <c r="O26" s="6">
         <v>1.8685338759839E-2</v>
       </c>
-      <c r="O26" s="6">
+      <c r="P26" s="6">
         <v>2.7956887186247802E-2</v>
       </c>
-      <c r="P26" s="6">
+      <c r="Q26" s="6">
         <v>0.66836263405714402</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="R26" s="6">
         <v>0.506232967950767</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>94</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>1.8685338759839003E-2</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>2.8161586269288736E-2</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>0.66350448377320514</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>0.50942826600190094</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -13764,53 +13801,54 @@
         <v>0.21681972818089901</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" t="s">
+      <c r="G27" s="6"/>
+      <c r="H27" t="s">
         <v>95</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>6.6802137047705346</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>5.4767209137332609</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>1.2197469635561364</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>0.22710748057151928</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>41</v>
       </c>
-      <c r="N27" s="6">
+      <c r="O27" s="6">
         <v>1.1732287972723E-2</v>
       </c>
-      <c r="O27" s="6">
+      <c r="P27" s="6">
         <v>3.2896779992766897E-2</v>
       </c>
-      <c r="P27" s="6">
+      <c r="Q27" s="6">
         <v>0.35663940286260898</v>
       </c>
-      <c r="Q27" s="6">
+      <c r="R27" s="6">
         <v>0.72249945117350201</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>95</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>1.1732287972722973E-2</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>3.3137648750960744E-2</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>0.35404708586582578</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>0.72448582066622014</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -13827,23 +13865,24 @@
         <v>0.98430024750457701</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="M28" t="s">
+      <c r="G28" s="6"/>
+      <c r="N28" t="s">
         <v>42</v>
       </c>
-      <c r="N28" s="6">
+      <c r="O28" s="6">
         <v>-1.3031615510313999E-2</v>
       </c>
-      <c r="O28" s="6">
+      <c r="P28" s="6">
         <v>3.12086257387802E-2</v>
       </c>
-      <c r="P28" s="6">
+      <c r="Q28" s="6">
         <v>-0.41756454191191</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="R28" s="6">
         <v>0.67762082405570401</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -13860,53 +13899,54 @@
         <v>0.80312156418173397</v>
       </c>
       <c r="F29" s="6"/>
-      <c r="G29" t="s">
+      <c r="G29" s="6"/>
+      <c r="H29" t="s">
         <v>96</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>-1.3409871324559073</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>5.4767209137332626</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>-0.2448521941465536</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>0.80736665929023754</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>43</v>
       </c>
-      <c r="N29" s="6">
+      <c r="O29" s="6">
         <v>2.0887824726044502E-2</v>
       </c>
-      <c r="O29" s="6">
+      <c r="P29" s="6">
         <v>3.2896779992766897E-2</v>
       </c>
-      <c r="P29" s="6">
+      <c r="Q29" s="6">
         <v>0.63495043377002802</v>
       </c>
-      <c r="Q29" s="6">
+      <c r="R29" s="6">
         <v>0.52765588116031004</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>96</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>2.0887824726044502E-2</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>3.3137648750960751E-2</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>0.63033514788640232</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>0.53075516481321139</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -13923,53 +13963,54 @@
         <v>9.0467702926530794E-2</v>
       </c>
       <c r="F30" s="6"/>
-      <c r="G30" t="s">
+      <c r="G30" s="6"/>
+      <c r="H30" t="s">
         <v>97</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>8.7318604745816515</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>5.1956736589426944</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>1.6806021793829449</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>9.7792419393728666E-2</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>44</v>
       </c>
-      <c r="N30" s="6">
+      <c r="O30" s="6">
         <v>2.0578482236366501E-2</v>
       </c>
-      <c r="O30" s="6">
+      <c r="P30" s="6">
         <v>3.12086257387802E-2</v>
       </c>
-      <c r="P30" s="6">
+      <c r="Q30" s="6">
         <v>0.65938444097509297</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="R30" s="6">
         <v>0.51194319301494495</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>97</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>2.0578482236366484E-2</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>3.1437133906700936E-2</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>0.65459155078956188</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>0.51511354277405186</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -13986,53 +14027,54 @@
         <v>0.67557115913499199</v>
       </c>
       <c r="F31" s="6"/>
-      <c r="G31" t="s">
+      <c r="G31" s="6"/>
+      <c r="H31" t="s">
         <v>124</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>-2.7170521218343566</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>6.6074670114507992</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>-0.41120933591127751</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>0.68231453440350309</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="6">
+      <c r="O31" s="6">
         <v>-2.93493724345451E-2</v>
       </c>
-      <c r="O31" s="6">
+      <c r="P31" s="6">
         <v>3.9688783125703099E-2</v>
       </c>
-      <c r="P31" s="6">
+      <c r="Q31" s="6">
         <v>-0.73948783820328401</v>
       </c>
-      <c r="Q31" s="6">
+      <c r="R31" s="6">
         <v>0.462232965617631</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>124</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>-2.9349372434545131E-2</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <v>3.9979382628384359E-2</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>-0.73411269772104515</v>
       </c>
-      <c r="W31">
+      <c r="X31">
         <v>0.46560355030411466</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -14049,53 +14091,54 @@
         <v>0.95515878597181803</v>
       </c>
       <c r="F32" s="6"/>
-      <c r="G32" t="s">
+      <c r="G32" s="6"/>
+      <c r="H32" t="s">
         <v>125</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>0.3764614236710373</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>6.8184625502184231</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>5.5212068834927852E-2</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>0.9561442378929853</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="6">
+      <c r="O32" s="6">
         <v>-2.6790726149040399E-4</v>
       </c>
-      <c r="O32" s="6">
+      <c r="P32" s="6">
         <v>4.09561608007072E-2</v>
       </c>
-      <c r="P32" s="6">
+      <c r="Q32" s="6">
         <v>-6.5413177468962797E-3</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="R32" s="6">
         <v>0.99480055281438395</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>125</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>-2.6790726149039689E-4</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <v>4.125603998628781E-2</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>-6.4937706473874061E-3</v>
       </c>
-      <c r="W32">
+      <c r="X32">
         <v>0.9948392765368721</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -14112,53 +14155,54 @@
         <v>0.13662358948439801</v>
       </c>
       <c r="F33" s="6"/>
-      <c r="G33" t="s">
+      <c r="G33" s="6"/>
+      <c r="H33" t="s">
         <v>126</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>9.9596535956981711</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>6.7570890013283158</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>1.4739562544966172</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>0.14547291423555067</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>58</v>
       </c>
-      <c r="N33" s="6">
+      <c r="O33" s="6">
         <v>4.2131661913300297E-2</v>
       </c>
-      <c r="O33" s="6">
+      <c r="P33" s="6">
         <v>4.0587510988709198E-2</v>
       </c>
-      <c r="P33" s="6">
+      <c r="Q33" s="6">
         <v>1.03804497706254</v>
       </c>
-      <c r="Q33" s="6">
+      <c r="R33" s="6">
         <v>0.30303725437492501</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>126</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>4.2131661913300297E-2</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <v>4.0884690936782576E-2</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>1.0304997041177548</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>0.30671554183697042</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -14175,53 +14219,54 @@
         <v>0.61082491583855303</v>
       </c>
       <c r="F34" s="6"/>
-      <c r="G34" t="s">
+      <c r="G34" s="6"/>
+      <c r="H34" t="s">
         <v>128</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>-3.9380085765654056</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>7.8732823776559764</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>-0.50017367441834648</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>0.61869550092109316</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>59</v>
       </c>
-      <c r="N34" s="6">
+      <c r="O34" s="6">
         <v>-1.5983525492887701E-2</v>
       </c>
-      <c r="O34" s="6">
+      <c r="P34" s="6">
         <v>4.7292100926523799E-2</v>
       </c>
-      <c r="P34" s="6">
+      <c r="Q34" s="6">
         <v>-0.33797452808706502</v>
       </c>
-      <c r="Q34" s="6">
+      <c r="R34" s="6">
         <v>0.736455073633836</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>128</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>-1.5983525492887715E-2</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>4.7638371583562454E-2</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>-0.33551788110244318</v>
       </c>
-      <c r="W34">
+      <c r="X34">
         <v>0.73834921608549253</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -14238,53 +14283,54 @@
         <v>6.1598607502696003E-2</v>
       </c>
       <c r="F35" s="6"/>
-      <c r="G35" t="s">
+      <c r="G35" s="6"/>
+      <c r="H35" t="s">
         <v>127</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>13.226179131822168</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>7.1107038953326729</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>1.8600379549630204</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>6.7549772374648265E-2</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>60</v>
       </c>
-      <c r="N35" s="6">
+      <c r="O35" s="6">
         <v>7.7783046352575297E-2</v>
       </c>
-      <c r="O35" s="6">
+      <c r="P35" s="6">
         <v>4.2711554107476998E-2</v>
       </c>
-      <c r="P35" s="6">
+      <c r="Q35" s="6">
         <v>1.82112423623936</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="R35" s="6">
         <v>7.3120780208466796E-2</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>127</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>7.7783046352575255E-2</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <v>4.30242862046811E-2</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>1.8078869683632859</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>7.5397938639559015E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -14301,58 +14347,59 @@
         <v>0.25373448308222801</v>
       </c>
       <c r="F36" s="6"/>
-      <c r="G36" t="s">
+      <c r="G36" s="6"/>
+      <c r="H36" t="s">
         <v>129</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>-8.6500413492625228</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>7.6804380214682944</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>-1.1262432331442558</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>0.26433447425299866</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>66</v>
       </c>
-      <c r="N36" s="6">
+      <c r="O36" s="6">
         <v>-4.3075505327091701E-2</v>
       </c>
-      <c r="O36" s="6">
+      <c r="P36" s="6">
         <v>4.6133751166095999E-2</v>
       </c>
-      <c r="P36" s="6">
+      <c r="Q36" s="6">
         <v>-0.93370914435304297</v>
       </c>
-      <c r="Q36" s="6">
+      <c r="R36" s="6">
         <v>0.35385743446773799</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>129</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>-4.3075505327091645E-2</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <v>4.6471540437770791E-2</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>-0.92692226083560292</v>
       </c>
-      <c r="W36">
+      <c r="X36">
         <v>0.35750438799522793</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="M20:Q20"/>
+    <mergeCell ref="N20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14364,7 +14411,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14375,10 +14422,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -14412,7 +14459,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -14702,7 +14749,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H13" t="s">
         <v>0</v>
@@ -14787,7 +14834,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -15030,7 +15077,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B27">
         <v>3.5507075436640649</v>
@@ -15113,12 +15160,12 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -15167,7 +15214,7 @@
         <v>0.17576629921828466</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H34" t="s">
         <v>0</v>
@@ -15378,7 +15425,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
@@ -15536,11 +15583,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -15712,7 +15759,7 @@
       <c r="D7" s="6">
         <v>5.0225586693001425</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="18">
         <v>1.7790570248084898E-6</v>
       </c>
       <c r="G7" t="s">
@@ -15744,7 +15791,7 @@
       <c r="D8" s="6">
         <v>2.3728957461317703</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="18">
         <v>1.922486649561269E-2</v>
       </c>
       <c r="G8" t="s">
@@ -15936,7 +15983,7 @@
       <c r="D14" s="6">
         <v>-3.2011237102050472</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="18">
         <v>1.7488789219186297E-3</v>
       </c>
       <c r="G14" t="s">
@@ -16000,7 +16047,7 @@
       <c r="D16" s="6">
         <v>4.2392253752478943</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="18">
         <v>4.4077972466853116E-5</v>
       </c>
       <c r="G16" t="s">
@@ -16032,7 +16079,7 @@
       <c r="D17" s="6">
         <v>3.3493775358785878</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="18">
         <v>1.0804075814037665E-3</v>
       </c>
       <c r="G17" t="s">
@@ -16084,11 +16131,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -16196,7 +16243,7 @@
       <c r="D25" s="6">
         <v>5.0225586693001416</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="18">
         <v>1.7790570248084965E-6</v>
       </c>
       <c r="G25" t="s">
@@ -16292,7 +16339,7 @@
       <c r="D28" s="6">
         <v>4.7310773684452023</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="18">
         <v>6.1088857379585714E-6</v>
       </c>
       <c r="G28" t="s">
@@ -16420,7 +16467,7 @@
       <c r="D32" s="6">
         <v>-3.2011237102050454</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="18">
         <v>1.7488789219186379E-3</v>
       </c>
       <c r="G32" t="s">
@@ -16484,7 +16531,7 @@
       <c r="D34" s="6">
         <v>3.6508568439997711</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="18">
         <v>3.8724155618843599E-4</v>
       </c>
       <c r="G34" t="s">
@@ -16516,7 +16563,7 @@
       <c r="D35" s="6">
         <v>3.1042897863681529</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="18">
         <v>2.375468357165829E-3</v>
       </c>
       <c r="G35" t="s">
@@ -16646,7 +16693,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16657,11 +16704,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -16825,11 +16872,11 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -16989,11 +17036,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -17223,11 +17270,11 @@
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -17468,7 +17515,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17482,12 +17529,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:14" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17507,7 +17554,7 @@
       <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>8.4827723785348087E-4</v>
       </c>
       <c r="D3" t="s">
@@ -17521,7 +17568,7 @@
       <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2.5573249466384537E-31</v>
       </c>
       <c r="D4" t="s">
@@ -17535,7 +17582,7 @@
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>9.9096899770360542E-5</v>
       </c>
       <c r="D5" t="s">
@@ -17549,7 +17596,7 @@
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <f>1/10000</f>
         <v>1E-4</v>
       </c>
@@ -17717,8 +17764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:F65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17732,11 +17779,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -17784,7 +17831,7 @@
       <c r="E3" s="6">
         <v>6.8476448906856882E-83</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
         <v>4</v>
@@ -17815,10 +17862,10 @@
       <c r="D4" s="6">
         <v>3.7025982312353865</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="18">
         <v>3.1331650862026381E-4</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="19"/>
       <c r="H4" t="s">
         <v>105</v>
       </c>
@@ -17848,10 +17895,10 @@
       <c r="D5" s="6">
         <v>3.024310317069947</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="18">
         <v>2.9994818416794007E-3</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="20"/>
       <c r="H5" t="s">
         <v>106</v>
       </c>
@@ -17881,10 +17928,10 @@
       <c r="D6" s="6">
         <v>7.944386363811569</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="18">
         <v>7.8263498735992003E-13</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3"/>
       <c r="H6" t="s">
         <v>92</v>
@@ -17915,10 +17962,10 @@
       <c r="D7" s="6">
         <v>4.1488439089952518</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="18">
         <v>5.9726584202964396E-5</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="21"/>
       <c r="H7" t="s">
         <v>93</v>
       </c>
@@ -17951,7 +17998,7 @@
       <c r="E8" s="6">
         <v>0.66364908711553217</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="20"/>
       <c r="H8" t="s">
         <v>94</v>
       </c>
@@ -17984,7 +18031,7 @@
       <c r="E9" s="6">
         <v>0.58049315316905858</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="20"/>
       <c r="H9" t="s">
         <v>96</v>
       </c>
@@ -18005,19 +18052,19 @@
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="18">
         <v>-345.00471099408134</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="18">
         <v>58.199900153131743</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="18">
         <v>-5.9279261663048848</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="18">
         <v>2.5617511159882357E-8</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="20"/>
       <c r="H10" t="s">
         <v>98</v>
       </c>
@@ -18050,7 +18097,7 @@
       <c r="E11" s="6">
         <v>0.34616907888281573</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="21"/>
       <c r="H11" t="s">
         <v>107</v>
       </c>
@@ -18080,10 +18127,10 @@
       <c r="D12" s="6">
         <v>2.5050192683066479</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="18">
         <v>1.3470832207404887E-2</v>
       </c>
-      <c r="F12" s="19"/>
+      <c r="F12" s="20"/>
       <c r="H12" t="s">
         <v>108</v>
       </c>
@@ -18113,10 +18160,10 @@
       <c r="D13" s="6">
         <v>-3.6094401114510792</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="18">
         <v>4.3552294070361525E-4</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="20"/>
       <c r="H13" t="s">
         <v>99</v>
       </c>
@@ -18149,7 +18196,7 @@
       <c r="E14" s="6">
         <v>7.3796863466524351E-2</v>
       </c>
-      <c r="F14" s="20"/>
+      <c r="F14" s="21"/>
       <c r="H14" t="s">
         <v>100</v>
       </c>
@@ -18182,7 +18229,7 @@
       <c r="E15" s="6">
         <v>0.19381122451147587</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="20"/>
       <c r="H15" t="s">
         <v>101</v>
       </c>
@@ -18215,7 +18262,7 @@
       <c r="E16" s="6">
         <v>0.32588118321571224</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="20"/>
       <c r="H16" t="s">
         <v>103</v>
       </c>
@@ -18237,14 +18284,14 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="19"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="19" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -18322,7 +18369,7 @@
       <c r="D22" s="6">
         <v>7.9443863638115682</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="18">
         <v>7.8263498735992003E-13</v>
       </c>
       <c r="F22" s="6"/>
@@ -18355,7 +18402,7 @@
       <c r="D23" s="6">
         <v>4.1488439089952491</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="18">
         <v>5.9726584202965006E-5</v>
       </c>
       <c r="F23" s="6"/>
@@ -18388,7 +18435,7 @@
       <c r="D24" s="6">
         <v>3.9869454505627306</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="18">
         <v>1.1061696628946535E-4</v>
       </c>
       <c r="F24" s="6"/>
@@ -18421,7 +18468,7 @@
       <c r="D25" s="6">
         <v>3.0243103170699435</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="18">
         <v>2.9994818416794332E-3</v>
       </c>
       <c r="F25" s="6"/>
@@ -18454,7 +18501,7 @@
       <c r="D26" s="6">
         <v>3.3456948661822397</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="18">
         <v>1.0711197146456059E-3</v>
       </c>
       <c r="F26" s="6"/>
@@ -18487,7 +18534,7 @@
       <c r="D27" s="6">
         <v>3.7025982312353847</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="18">
         <v>3.1331650862026522E-4</v>
       </c>
       <c r="F27" s="6"/>
@@ -18520,10 +18567,10 @@
       <c r="D28" s="6">
         <v>-5.9279261663048857</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="18">
         <v>2.5617511159882205E-8</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="18"/>
       <c r="G28" s="2"/>
       <c r="H28" t="s">
         <v>98</v>
@@ -18554,7 +18601,7 @@
       <c r="D29" s="6">
         <v>-3.6094401114510766</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="18">
         <v>4.3552294070361888E-4</v>
       </c>
       <c r="F29" s="6"/>
@@ -18653,7 +18700,7 @@
       <c r="D32" s="6">
         <v>2.5050192683066506</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="18">
         <v>1.347083220740479E-2</v>
       </c>
       <c r="F32" s="6"/>
@@ -18752,463 +18799,729 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F30"/>
+  <dimension ref="A2:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1338.3786022420861</v>
+      </c>
+      <c r="C3">
+        <v>23.386706046603653</v>
+      </c>
+      <c r="D3">
+        <v>57.228179102052422</v>
+      </c>
+      <c r="E3">
+        <v>4.9396824791406674E-56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>1683.3833132361676</v>
+      </c>
+      <c r="J3">
+        <v>44.413781225167291</v>
+      </c>
+      <c r="K3">
+        <v>37.902274177058132</v>
+      </c>
+      <c r="L3">
+        <v>7.070829550210474E-53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>236.87871396784379</v>
+      </c>
+      <c r="C4">
+        <v>41.835411592008917</v>
+      </c>
+      <c r="D4">
+        <v>5.6621580845900068</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.9497517062357979E-7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4">
+        <v>229.56811863214338</v>
+      </c>
+      <c r="J4">
+        <v>75.488912379856302</v>
+      </c>
+      <c r="K4">
+        <v>3.0410839339818341</v>
+      </c>
+      <c r="L4" s="2">
+        <v>3.1864065625701221E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>213.99626455778031</v>
+      </c>
+      <c r="C5">
+        <v>37.502160613536581</v>
+      </c>
+      <c r="D5">
+        <v>5.7062382821894628</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.331143813140082E-7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5">
+        <v>15.822569116773366</v>
+      </c>
+      <c r="J5">
+        <v>188.43171529470936</v>
+      </c>
+      <c r="K5">
+        <v>8.3969777019896497E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.93329022995139721</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6">
+        <v>127.96729625070191</v>
+      </c>
+      <c r="C6">
+        <v>33.073796870339748</v>
+      </c>
+      <c r="D6">
+        <v>3.8691444091640323</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.6162844142097618E-4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6">
+        <v>431.23773156183893</v>
+      </c>
+      <c r="J6">
+        <v>66.089821371171894</v>
+      </c>
+      <c r="K6">
+        <v>6.5250249223694077</v>
+      </c>
+      <c r="L6" s="2">
+        <v>5.7094921661119859E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7">
+        <v>78.835972072487849</v>
+      </c>
+      <c r="C7">
+        <v>37.502160613536581</v>
+      </c>
+      <c r="D7">
+        <v>2.1021714691294782</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3.9541462868423451E-2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7">
+        <v>248.68440089332032</v>
+      </c>
+      <c r="J7">
+        <v>72.979289523370696</v>
+      </c>
+      <c r="K7">
+        <v>3.4076023830525548</v>
+      </c>
+      <c r="L7">
+        <v>1.0283311764847521E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1338.3786022420861</v>
-      </c>
-      <c r="C4">
-        <v>23.386706046603653</v>
-      </c>
-      <c r="D4">
-        <v>57.228179102052422</v>
-      </c>
-      <c r="E4">
-        <v>4.9396824791406674E-56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5">
-        <v>236.87871396784379</v>
-      </c>
-      <c r="C5">
+      <c r="B8">
+        <v>109.97854061505643</v>
+      </c>
+      <c r="C8">
+        <v>81.013926188791615</v>
+      </c>
+      <c r="D8">
+        <v>1.3575263635386197</v>
+      </c>
+      <c r="E8">
+        <v>0.17945709000962828</v>
+      </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8">
+        <v>-26.763598772996168</v>
+      </c>
+      <c r="J8">
+        <v>74.759533802485024</v>
+      </c>
+      <c r="K8">
+        <v>-0.35799579547547339</v>
+      </c>
+      <c r="L8">
+        <v>0.72128932028960491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9">
+        <v>3.0933805932666241</v>
+      </c>
+      <c r="C9">
+        <v>44.218812969867663</v>
+      </c>
+      <c r="D9">
+        <v>6.9956210615028686E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.94445009835469795</v>
+      </c>
+      <c r="H9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9">
+        <v>145.31443211126103</v>
+      </c>
+      <c r="J9">
+        <v>189.12832290256091</v>
+      </c>
+      <c r="K9">
+        <v>0.76833776073891991</v>
+      </c>
+      <c r="L9">
+        <v>0.44454873493887093</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>190.26599858474856</v>
+      </c>
+      <c r="C10">
+        <v>45.41737194439802</v>
+      </c>
+      <c r="D10">
+        <v>4.1892780325924779</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8.8755130112118128E-5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10">
+        <v>50.075908749818893</v>
+      </c>
+      <c r="J10">
+        <v>110.0430541702835</v>
+      </c>
+      <c r="K10">
+        <v>0.45505742390910131</v>
+      </c>
+      <c r="L10">
+        <v>0.65030048696362708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11">
+        <v>-161.33860138707749</v>
+      </c>
+      <c r="C11">
+        <v>49.056368462464597</v>
+      </c>
+      <c r="D11">
+        <v>-3.288841111639266</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.6489175335300582E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12">
+        <v>-91.64834772852511</v>
+      </c>
+      <c r="C12">
         <v>41.835411592008917</v>
       </c>
-      <c r="D5">
-        <v>5.6621580845900068</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3.9497517062357979E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6">
-        <v>213.99626455778031</v>
-      </c>
-      <c r="C6">
-        <v>37.502160613536581</v>
-      </c>
-      <c r="D6">
-        <v>5.7062382821894628</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3.331143813140082E-7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7">
-        <v>127.96729625070191</v>
-      </c>
-      <c r="C7">
-        <v>33.073796870339748</v>
-      </c>
-      <c r="D7">
-        <v>3.8691444091640323</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.6162844142097618E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8">
-        <v>78.835972072487849</v>
-      </c>
-      <c r="C8">
-        <v>37.502160613536581</v>
-      </c>
-      <c r="D8">
-        <v>2.1021714691294782</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3.9541462868423451E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D12">
+        <v>-2.1906883245779056</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3.2182052386035574E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>139</v>
       </c>
-      <c r="B9">
-        <v>109.97854061505643</v>
-      </c>
-      <c r="C9">
-        <v>81.013926188791615</v>
-      </c>
-      <c r="D9">
-        <v>1.3575263635386197</v>
-      </c>
-      <c r="E9">
-        <v>0.17945709000962828</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10">
-        <v>3.0933805932666241</v>
-      </c>
-      <c r="C10">
-        <v>44.218812969867663</v>
-      </c>
-      <c r="D10">
-        <v>6.9956210615028686E-2</v>
-      </c>
-      <c r="E10">
-        <v>0.94445009835469795</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11">
-        <v>190.26599858474856</v>
-      </c>
-      <c r="C11">
-        <v>45.41737194439802</v>
-      </c>
-      <c r="D11">
-        <v>4.1892780325924779</v>
-      </c>
-      <c r="E11" s="2">
-        <v>8.8755130112118128E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12">
-        <v>-161.33860138707749</v>
-      </c>
-      <c r="C12">
-        <v>49.056368462464597</v>
-      </c>
-      <c r="D12">
-        <v>-3.288841111639266</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.6489175335300582E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
       <c r="B13">
-        <v>-91.64834772852511</v>
+        <v>72.492683790069762</v>
       </c>
       <c r="C13">
-        <v>41.835411592008917</v>
+        <v>64.895475587816662</v>
       </c>
       <c r="D13">
-        <v>-2.1906883245779056</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3.2182052386035574E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.1170683800902661</v>
+      </c>
+      <c r="E13">
+        <v>0.26820722175796674</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>140</v>
       </c>
       <c r="B14">
-        <v>72.492683790069762</v>
+        <v>39.557007397496776</v>
       </c>
       <c r="C14">
         <v>64.895475587816662</v>
       </c>
       <c r="D14">
-        <v>1.1170683800902661</v>
+        <v>0.60954954161585839</v>
       </c>
       <c r="E14">
-        <v>0.26820722175796674</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15">
-        <v>39.557007397496776</v>
-      </c>
-      <c r="C15">
-        <v>64.895475587816662</v>
-      </c>
-      <c r="D15">
-        <v>0.60954954161585839</v>
-      </c>
-      <c r="E15">
         <v>0.54435243368619524</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D17" t="s">
         <v>2</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>1338.3786022420861</v>
+      </c>
+      <c r="C18">
+        <v>23.386706046603653</v>
+      </c>
+      <c r="D18">
+        <v>57.228179102052422</v>
+      </c>
+      <c r="E18">
+        <v>4.9396824791406674E-56</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1683.3833132361672</v>
+      </c>
+      <c r="J18">
+        <v>44.413781225167298</v>
+      </c>
+      <c r="K18">
+        <v>37.902274177058118</v>
+      </c>
+      <c r="L18">
+        <v>7.0708295502105741E-53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="B19">
-        <v>1338.3786022420861</v>
+        <v>127.96729625070195</v>
       </c>
       <c r="C19">
-        <v>23.386706046603653</v>
+        <v>33.073796870339756</v>
       </c>
       <c r="D19">
-        <v>57.228179102052422</v>
-      </c>
-      <c r="E19">
-        <v>4.9396824791406674E-56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.8691444091640328</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2.6162844142097613E-4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19">
+        <v>431.23773156183881</v>
+      </c>
+      <c r="J19">
+        <v>66.089821371171894</v>
+      </c>
+      <c r="K19">
+        <v>6.5250249223694059</v>
+      </c>
+      <c r="L19" s="2">
+        <v>5.7094921661120272E-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B20">
-        <v>127.96729625070195</v>
+        <v>78.835972072487834</v>
       </c>
       <c r="C20">
-        <v>33.073796870339756</v>
+        <v>37.502160613536581</v>
       </c>
       <c r="D20">
-        <v>3.8691444091640328</v>
+        <v>2.1021714691294777</v>
       </c>
       <c r="E20" s="2">
-        <v>2.6162844142097613E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.9541462868423485E-2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20">
+        <v>248.68440089332032</v>
+      </c>
+      <c r="J20">
+        <v>72.979289523370696</v>
+      </c>
+      <c r="K20">
+        <v>3.4076023830525548</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1.0283311764847521E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="B21">
-        <v>78.835972072487834</v>
+        <v>109.9785406150564</v>
       </c>
       <c r="C21">
-        <v>37.502160613536581</v>
+        <v>81.013926188791601</v>
       </c>
       <c r="D21">
-        <v>2.1021714691294777</v>
-      </c>
-      <c r="E21" s="2">
-        <v>3.9541462868423485E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.3575263635386197</v>
+      </c>
+      <c r="E21">
+        <v>0.17945709000962828</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="H21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21">
+        <v>202.80451985914715</v>
+      </c>
+      <c r="J21">
+        <v>61.932058963878504</v>
+      </c>
+      <c r="K21">
+        <v>3.2746290572614685</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.564656229163624E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22">
+        <v>239.9720945611104</v>
+      </c>
+      <c r="C22">
+        <v>36.041334559250707</v>
+      </c>
+      <c r="D22">
+        <v>6.6582466353071519</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7.8476194379247186E-9</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="H22" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22">
+        <v>161.13700122803442</v>
+      </c>
+      <c r="J22">
+        <v>64.870479576329515</v>
+      </c>
+      <c r="K22">
+        <v>2.4839804219180066</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.5080988422936962E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23">
+        <v>404.26226314252892</v>
+      </c>
+      <c r="C23">
+        <v>41.835411592008903</v>
+      </c>
+      <c r="D23">
+        <v>9.6631596955472094</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4.6873235494355556E-14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>133</v>
+      </c>
+      <c r="I23">
+        <v>15.822569116773339</v>
+      </c>
+      <c r="J23">
+        <v>188.43171529470942</v>
+      </c>
+      <c r="K23">
+        <v>8.396977701989633E-2</v>
+      </c>
+      <c r="L23">
+        <v>0.93329022995139732</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24">
+        <v>213.99626455778039</v>
+      </c>
+      <c r="C24">
+        <v>37.502160613536589</v>
+      </c>
+      <c r="D24">
+        <v>5.7062382821894637</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3.331143813140082E-7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24">
+        <v>279.64402738196225</v>
+      </c>
+      <c r="J24">
+        <v>101.76475718176883</v>
+      </c>
+      <c r="K24">
+        <v>2.7479457046457783</v>
+      </c>
+      <c r="L24" s="2">
+        <v>7.4084951004470762E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25">
+        <v>75.540112580766305</v>
+      </c>
+      <c r="C25">
+        <v>41.835411592008903</v>
+      </c>
+      <c r="D25">
+        <v>1.8056500391930035</v>
+      </c>
+      <c r="E25">
+        <v>7.5750955551022292E-2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25">
+        <v>229.56811863214338</v>
+      </c>
+      <c r="J25">
+        <v>75.488912379856316</v>
+      </c>
+      <c r="K25">
+        <v>3.0410839339818336</v>
+      </c>
+      <c r="L25" s="2">
+        <v>3.186406562570126E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26">
+        <v>145.2303662393187</v>
+      </c>
+      <c r="C26">
+        <v>33.073796870339763</v>
+      </c>
+      <c r="D26">
+        <v>4.3911005080145422</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.3967746987810889E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>139</v>
       </c>
-      <c r="B22">
-        <v>109.9785406150564</v>
-      </c>
-      <c r="C22">
-        <v>81.013926188791601</v>
-      </c>
-      <c r="D22">
-        <v>1.3575263635386197</v>
-      </c>
-      <c r="E22">
-        <v>0.17945709000962828</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23">
-        <v>239.9720945611104</v>
-      </c>
-      <c r="C23">
-        <v>36.041334559250707</v>
-      </c>
-      <c r="D23">
-        <v>6.6582466353071519</v>
-      </c>
-      <c r="E23" s="2">
-        <v>7.8476194379247186E-9</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24">
-        <v>404.26226314252892</v>
-      </c>
-      <c r="C24">
-        <v>41.835411592008903</v>
-      </c>
-      <c r="D24">
-        <v>9.6631596955472094</v>
-      </c>
-      <c r="E24" s="2">
-        <v>4.6873235494355556E-14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25">
-        <v>213.99626455778039</v>
-      </c>
-      <c r="C25">
-        <v>37.502160613536589</v>
-      </c>
-      <c r="D25">
-        <v>5.7062382821894637</v>
-      </c>
-      <c r="E25" s="2">
-        <v>3.331143813140082E-7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26">
-        <v>75.540112580766305</v>
-      </c>
-      <c r="C26">
-        <v>41.835411592008903</v>
-      </c>
-      <c r="D26">
-        <v>1.8056500391930035</v>
-      </c>
-      <c r="E26">
-        <v>7.5750955551022292E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
       <c r="B27">
-        <v>145.2303662393187</v>
+        <v>309.3713977579136</v>
       </c>
       <c r="C27">
-        <v>33.073796870339763</v>
+        <v>59.624635245145214</v>
       </c>
       <c r="D27">
-        <v>4.3911005080145422</v>
+        <v>5.1886505717970559</v>
       </c>
       <c r="E27" s="2">
-        <v>4.3967746987810889E-5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.4010311086635611E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>140</v>
       </c>
       <c r="B28">
-        <v>309.3713977579136</v>
+        <v>276.43572136534056</v>
       </c>
       <c r="C28">
-        <v>59.624635245145214</v>
+        <v>59.624635245145207</v>
       </c>
       <c r="D28">
-        <v>5.1886505717970559</v>
+        <v>4.6362668757432557</v>
       </c>
       <c r="E28" s="2">
-        <v>2.4010311086635611E-6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.8367392490764613E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B29">
-        <v>276.43572136534056</v>
+        <v>236.87871396784379</v>
       </c>
       <c r="C29">
-        <v>59.624635245145207</v>
+        <v>41.83541159200891</v>
       </c>
       <c r="D29">
-        <v>4.6362668757432557</v>
+        <v>5.6621580845900086</v>
       </c>
       <c r="E29" s="2">
-        <v>1.8367392490764613E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30">
-        <v>236.87871396784379</v>
-      </c>
-      <c r="C30">
-        <v>41.83541159200891</v>
-      </c>
-      <c r="D30">
-        <v>5.6621580845900086</v>
-      </c>
-      <c r="E30" s="2">
         <v>3.9497517062357539E-7</v>
       </c>
     </row>
@@ -19222,7 +19535,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19236,13 +19549,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -19259,7 +19572,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B3">
@@ -19274,10 +19587,10 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1.1225128823082477E-11</v>
       </c>
       <c r="D4" t="s">
@@ -19289,10 +19602,10 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>2.9885590415854351E-2</v>
       </c>
       <c r="D5" t="s">
@@ -19304,7 +19617,7 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B6">
@@ -19450,7 +19763,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19460,11 +19773,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -19732,7 +20045,7 @@
       <c r="D10">
         <v>-3.4586133196803441</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1.3279127300325946E-3</v>
       </c>
       <c r="G10" t="s">
@@ -19912,11 +20225,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -20184,7 +20497,7 @@
       <c r="D26">
         <v>-3.4586133196803419</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>1.327912730032603E-3</v>
       </c>
       <c r="G26" t="s">
@@ -20375,10 +20688,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20389,10 +20702,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -20466,7 +20779,7 @@
       <c r="D4">
         <v>2.9446990238552044</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1.1387246418000671E-2</v>
       </c>
       <c r="H4" t="s">
@@ -20498,7 +20811,7 @@
       <c r="D5">
         <v>2.5469331067816752</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>2.4333366085376253E-2</v>
       </c>
       <c r="H5" t="s">
@@ -20664,7 +20977,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -20679,7 +20992,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I13" t="s">
         <v>0</v>
@@ -20739,7 +21052,7 @@
       <c r="D15">
         <v>2.1107747592603099</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>5.4731001685439838E-2</v>
       </c>
       <c r="H15" t="s">
@@ -20803,7 +21116,7 @@
       <c r="D17">
         <v>2.8594760574601055</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>1.3411079933650408E-2</v>
       </c>
       <c r="H17" t="s">
@@ -20835,7 +21148,7 @@
       <c r="D18">
         <v>2.5469331067816752</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>2.4333366085376253E-2</v>
       </c>
       <c r="H18" t="s">
@@ -20867,7 +21180,7 @@
       <c r="D19">
         <v>2.653795923186697</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>1.9867753773916676E-2</v>
       </c>
       <c r="H19" t="s">
@@ -20899,7 +21212,7 @@
       <c r="D20">
         <v>2.1990876391998304</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>4.6575497414492732E-2</v>
       </c>
       <c r="H20" t="s">
@@ -20920,7 +21233,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21">
         <v>12.991499999999998</v>
@@ -20931,8 +21244,314 @@
       <c r="D21">
         <v>2.944699023855204</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>1.1387246418000678E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>86.399999999999977</v>
+      </c>
+      <c r="C26">
+        <v>4.9422896308019642</v>
+      </c>
+      <c r="D26">
+        <v>17.48177594884908</v>
+      </c>
+      <c r="E26">
+        <v>2.0600133579824691E-10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27">
+        <v>17.836111111111123</v>
+      </c>
+      <c r="C27">
+        <v>6.9894530250560551</v>
+      </c>
+      <c r="D27">
+        <v>2.5518607889875731</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.4107583030653384E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28">
+        <v>11.457142857142863</v>
+      </c>
+      <c r="C28">
+        <v>8.5602967462698309</v>
+      </c>
+      <c r="D28">
+        <v>1.3384048703843519</v>
+      </c>
+      <c r="E28">
+        <v>0.20370300436547595</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <v>9.4694444444444485</v>
+      </c>
+      <c r="C29">
+        <v>6.0530438782565374</v>
+      </c>
+      <c r="D29">
+        <v>1.5644103421189703</v>
+      </c>
+      <c r="E29">
+        <v>0.14172960015678773</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>9.0000000000000018</v>
+      </c>
+      <c r="C30">
+        <v>6.9894530250560551</v>
+      </c>
+      <c r="D30">
+        <v>1.2876544083974042</v>
+      </c>
+      <c r="E30">
+        <v>0.22031754188052113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31">
+        <v>-3.2898148148148105</v>
+      </c>
+      <c r="C31">
+        <v>6.3804684774098703</v>
+      </c>
+      <c r="D31">
+        <v>-0.51560709475525845</v>
+      </c>
+      <c r="E31">
+        <v>0.61478491773587418</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32">
+        <v>-4.204861111111116</v>
+      </c>
+      <c r="C32">
+        <v>6.0530438782565366</v>
+      </c>
+      <c r="D32">
+        <v>-0.6946688634152518</v>
+      </c>
+      <c r="E32">
+        <v>0.49949069839462945</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33">
+        <v>-5.8366123642439485</v>
+      </c>
+      <c r="C33">
+        <v>6.3804684774098703</v>
+      </c>
+      <c r="D33">
+        <v>-0.91476235403537354</v>
+      </c>
+      <c r="E33">
+        <v>0.3769718330862753</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>86.4</v>
+      </c>
+      <c r="C37">
+        <v>4.942289630801965</v>
+      </c>
+      <c r="D37">
+        <v>17.481775948849084</v>
+      </c>
+      <c r="E37">
+        <v>2.0600133579824691E-10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38">
+        <v>9.4694444444444432</v>
+      </c>
+      <c r="C38">
+        <v>6.0530438782565366</v>
+      </c>
+      <c r="D38">
+        <v>1.5644103421189697</v>
+      </c>
+      <c r="E38">
+        <v>0.1417296001567879</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39">
+        <v>8.9999999999999982</v>
+      </c>
+      <c r="C39">
+        <v>6.9894530250560551</v>
+      </c>
+      <c r="D39">
+        <v>1.2876544083974037</v>
+      </c>
+      <c r="E39">
+        <v>0.22031754188052127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40">
+        <v>14.546296296296303</v>
+      </c>
+      <c r="C40">
+        <v>6.3804684774098694</v>
+      </c>
+      <c r="D40">
+        <v>2.2798163407275895</v>
+      </c>
+      <c r="E40" s="2">
+        <v>4.0132618926117962E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41">
+        <v>11.457142857142857</v>
+      </c>
+      <c r="C41">
+        <v>8.5602967462698309</v>
+      </c>
+      <c r="D41">
+        <v>1.3384048703843514</v>
+      </c>
+      <c r="E41">
+        <v>0.2037030043654762</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42">
+        <v>13.631249999999998</v>
+      </c>
+      <c r="C42">
+        <v>6.0530438782565366</v>
+      </c>
+      <c r="D42">
+        <v>2.2519661634975985</v>
+      </c>
+      <c r="E42" s="2">
+        <v>4.2253746079800959E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43">
+        <v>11.999498746867165</v>
+      </c>
+      <c r="C43">
+        <v>6.3804684774098703</v>
+      </c>
+      <c r="D43">
+        <v>1.880661081447474</v>
+      </c>
+      <c r="E43" s="2">
+        <v>8.2606882006138804E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44">
+        <v>17.836111111111112</v>
+      </c>
+      <c r="C44">
+        <v>6.9894530250560551</v>
+      </c>
+      <c r="D44">
+        <v>2.5518607889875713</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2.4107583030653478E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>